<commit_message>
nueva configuracion de grilla
</commit_message>
<xml_diff>
--- a/SANTA3/FORMULAss.xlsx
+++ b/SANTA3/FORMULAss.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9264"/>
+    <workbookView windowWidth="22368" windowHeight="9264" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="formula ganancias" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="115">
   <si>
     <t>SALDO INICIAL</t>
   </si>
@@ -39,13 +39,13 @@
     <t>GANANCIA TOTAL</t>
   </si>
   <si>
-    <t>1487</t>
-  </si>
-  <si>
-    <t>1.5</t>
-  </si>
-  <si>
-    <t>90</t>
+    <t>1514</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>365</t>
   </si>
   <si>
     <t>calculadora diaria</t>
@@ -141,7 +141,10 @@
     <t>margen ratio</t>
   </si>
   <si>
-    <t>1.7</t>
+    <t>2</t>
+  </si>
+  <si>
+    <t>15</t>
   </si>
   <si>
     <t>primer tp a 0.7 porciento</t>
@@ -201,6 +204,9 @@
     <t>muy movido</t>
   </si>
   <si>
+    <t>buena ganancia:</t>
+  </si>
+  <si>
     <t>ARCHIVO</t>
   </si>
   <si>
@@ -261,6 +267,12 @@
     <t>CCXT</t>
   </si>
   <si>
+    <t>a veces no consigue obtener el df y falla saliendo del updating en medio de un trade.</t>
+  </si>
+  <si>
+    <t>TESTING</t>
+  </si>
+  <si>
     <t>equipoliquidando</t>
   </si>
   <si>
@@ -340,6 +352,9 @@
   </si>
   <si>
     <t>formacioninicial</t>
+  </si>
+  <si>
+    <t>no crea la primera compensacion... se arregló dividiendo preciostopsanta por multiplier</t>
   </si>
   <si>
     <t>creaactualizatps</t>
@@ -359,11 +374,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
+    <numFmt numFmtId="176" formatCode="0.000000"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="0.000000"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="0.00000"/>
   </numFmts>
   <fonts count="27">
@@ -431,9 +446,24 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -443,6 +473,14 @@
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -462,15 +500,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -483,9 +513,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -496,6 +526,14 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -514,14 +552,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -530,23 +560,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -560,16 +582,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -614,7 +629,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -638,19 +653,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -662,37 +701,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -710,13 +731,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -728,13 +749,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -746,49 +797,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1037,17 +1052,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1100,6 +1111,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1114,38 +1149,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1155,175 +1170,176 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1491,7 +1507,7 @@
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1536,6 +1552,14 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1552,6 +1576,53 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>6985</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="616585" y="1438910"/>
+          <a:ext cx="8824595" cy="3422650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1843,87 +1914,87 @@
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="20.5740740740741" style="49" customWidth="1"/>
-    <col min="2" max="2" width="34.287037037037" style="49" customWidth="1"/>
-    <col min="3" max="3" width="14.1481481481481" style="50" customWidth="1"/>
-    <col min="4" max="4" width="21.8888888888889" style="20" customWidth="1"/>
-    <col min="5" max="5" width="17.1111111111111" style="20" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="20"/>
+    <col min="1" max="1" width="20.5740740740741" style="50" customWidth="1"/>
+    <col min="2" max="2" width="34.287037037037" style="50" customWidth="1"/>
+    <col min="3" max="3" width="14.1481481481481" style="51" customWidth="1"/>
+    <col min="4" max="4" width="21.8888888888889" style="21" customWidth="1"/>
+    <col min="5" max="5" width="17.1111111111111" style="21" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="21"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1" spans="1:5">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="52" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" ht="19.5" customHeight="1" spans="1:5">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="53">
+      <c r="D2" s="54">
         <f>POWER(1+(B2/100),C2)*A2</f>
-        <v>5678.77642796506</v>
-      </c>
-      <c r="E2" s="53">
+        <v>57204.1195799913</v>
+      </c>
+      <c r="E2" s="54">
         <f>D2-A2</f>
-        <v>4191.77642796506</v>
+        <v>55690.1195799913</v>
       </c>
     </row>
     <row r="3" ht="19.5" customHeight="1" spans="1:2">
-      <c r="A3" s="50"/>
-      <c r="B3" s="50"/>
+      <c r="A3" s="51"/>
+      <c r="B3" s="51"/>
     </row>
     <row r="4" ht="19.5" customHeight="1"/>
     <row r="5" ht="19.5" customHeight="1"/>
     <row r="6" ht="19.5" customHeight="1" spans="1:2">
-      <c r="A6" s="54"/>
-      <c r="B6" s="54"/>
+      <c r="A6" s="55"/>
+      <c r="B6" s="55"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="55"/>
+      <c r="B7" s="56"/>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="57" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="56">
+      <c r="B9" s="57">
         <f>A9*100/A2</f>
-        <v>1.68123739071957</v>
+        <v>1.65125495376486</v>
       </c>
     </row>
   </sheetData>
@@ -1947,425 +2018,425 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44444444444444" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22" style="19" customWidth="1"/>
-    <col min="2" max="2" width="12.8888888888889" style="19" customWidth="1"/>
-    <col min="3" max="3" width="27.7777777777778" style="19" customWidth="1"/>
-    <col min="4" max="4" width="8.44444444444444" style="19" customWidth="1"/>
-    <col min="5" max="5" width="18.5555555555556" style="19" customWidth="1"/>
-    <col min="6" max="6" width="17.1111111111111" style="19" customWidth="1"/>
-    <col min="7" max="7" width="15.6666666666667" style="19" customWidth="1"/>
-    <col min="8" max="8" width="1.66666666666667" style="19" customWidth="1"/>
-    <col min="9" max="9" width="32.8888888888889" style="19" customWidth="1"/>
-    <col min="10" max="10" width="31.2222222222222" style="19" customWidth="1"/>
-    <col min="11" max="11" width="8.44444444444444" style="19" customWidth="1"/>
-    <col min="12" max="12" width="31.2222222222222" style="19" customWidth="1"/>
-    <col min="13" max="16374" width="8.44444444444444" style="19" customWidth="1"/>
-    <col min="16375" max="16375" width="8.44444444444444" style="19"/>
-    <col min="16376" max="16384" width="8.44444444444444" style="20"/>
+    <col min="1" max="1" width="22" style="20" customWidth="1"/>
+    <col min="2" max="2" width="12.8888888888889" style="20" customWidth="1"/>
+    <col min="3" max="3" width="27.7777777777778" style="20" customWidth="1"/>
+    <col min="4" max="4" width="8.44444444444444" style="20" customWidth="1"/>
+    <col min="5" max="5" width="18.5555555555556" style="20" customWidth="1"/>
+    <col min="6" max="6" width="17.1111111111111" style="20" customWidth="1"/>
+    <col min="7" max="7" width="15.6666666666667" style="20" customWidth="1"/>
+    <col min="8" max="8" width="1.66666666666667" style="20" customWidth="1"/>
+    <col min="9" max="9" width="32.8888888888889" style="20" customWidth="1"/>
+    <col min="10" max="10" width="31.2222222222222" style="20" customWidth="1"/>
+    <col min="11" max="11" width="8.44444444444444" style="20" customWidth="1"/>
+    <col min="12" max="12" width="31.2222222222222" style="20" customWidth="1"/>
+    <col min="13" max="16374" width="8.44444444444444" style="20" customWidth="1"/>
+    <col min="16375" max="16375" width="8.44444444444444" style="20"/>
+    <col min="16376" max="16384" width="8.44444444444444" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" s="19" customFormat="1" ht="15.75" spans="1:2">
-      <c r="A1" s="21" t="s">
+    <row r="1" s="20" customFormat="1" ht="15.75" spans="1:2">
+      <c r="A1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="23" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" s="19" customFormat="1" ht="15.15" spans="4:7">
-      <c r="D2" s="23" t="s">
+    <row r="2" s="20" customFormat="1" ht="15.15" spans="4:7">
+      <c r="D2" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="27" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" s="19" customFormat="1" spans="1:10">
-      <c r="A3" s="27" t="s">
+    <row r="3" s="20" customFormat="1" spans="1:10">
+      <c r="A3" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="28">
+      <c r="B3" s="29">
         <v>1457</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="30">
+      <c r="E3" s="31">
         <f>G3/F3</f>
         <v>68.6339165545087</v>
       </c>
-      <c r="F3" s="31">
+      <c r="F3" s="32">
         <v>1.486</v>
       </c>
-      <c r="G3" s="32">
+      <c r="G3" s="33">
         <f>B8</f>
         <v>101.99</v>
       </c>
-      <c r="I3" s="27" t="s">
+      <c r="I3" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="42">
+      <c r="J3" s="43">
         <f>IF(B1="BUY",((I10/J10)-1)*-100,((I10/J10)-1)*100)</f>
         <v>-7.05645174826999</v>
       </c>
     </row>
-    <row r="4" s="19" customFormat="1" spans="1:10">
-      <c r="A4" s="27" t="s">
+    <row r="4" s="20" customFormat="1" spans="1:10">
+      <c r="A4" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="33">
+      <c r="B4" s="34">
         <f>-B3*$B$10/100</f>
         <v>-145.7</v>
       </c>
-      <c r="D4" s="34">
+      <c r="D4" s="35">
         <v>1</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="31">
         <f t="shared" ref="E4:E9" si="0">E3*(1+$B$6/100)</f>
         <v>89.2240915208614</v>
       </c>
-      <c r="F4" s="35">
+      <c r="F4" s="36">
         <f>IF($B$1="BUY",F3*(1-$B$5/100),F3*(1+$B$5/100))</f>
         <v>1.511262</v>
       </c>
-      <c r="G4" s="32">
+      <c r="G4" s="33">
         <f t="shared" ref="G4:G13" si="1">E4*F4</f>
         <v>134.840979</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="42">
+      <c r="J4" s="43">
         <f>E18</f>
         <v>1206.77910471736</v>
       </c>
     </row>
-    <row r="5" s="19" customFormat="1" spans="1:10">
-      <c r="A5" s="27" t="s">
+    <row r="5" s="20" customFormat="1" spans="1:10">
+      <c r="A5" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="33">
+      <c r="B5" s="34">
         <v>1.7</v>
       </c>
-      <c r="D5" s="34">
+      <c r="D5" s="35">
         <v>2</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="31">
         <f t="shared" si="0"/>
         <v>115.99131897712</v>
       </c>
-      <c r="F5" s="35">
+      <c r="F5" s="36">
         <f>IF($B$1="BUY",F4*(1-$B$5/100),F4*(1+$B$5/100))</f>
         <v>1.536953454</v>
       </c>
-      <c r="G5" s="32">
+      <c r="G5" s="33">
         <f t="shared" si="1"/>
         <v>178.2732583359</v>
       </c>
-      <c r="I5" s="27" t="s">
+      <c r="I5" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="42">
+      <c r="J5" s="43">
         <f>J4*J10</f>
         <v>2064.77710324769</v>
       </c>
     </row>
-    <row r="6" s="19" customFormat="1" spans="1:10">
-      <c r="A6" s="27" t="s">
+    <row r="6" s="20" customFormat="1" spans="1:10">
+      <c r="A6" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="33">
+      <c r="B6" s="34">
         <v>30</v>
       </c>
-      <c r="D6" s="34">
+      <c r="D6" s="35">
         <v>3</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="31">
         <f t="shared" si="0"/>
         <v>150.788714670256</v>
       </c>
-      <c r="F6" s="35">
+      <c r="F6" s="36">
         <f>IF($B$1="BUY",F5*(1-$B$5/100),F5*(1+$B$5/100))</f>
         <v>1.563081662718</v>
       </c>
-      <c r="G6" s="32">
+      <c r="G6" s="33">
         <f t="shared" si="1"/>
         <v>235.695074845893</v>
       </c>
-      <c r="I6" s="27" t="s">
+      <c r="I6" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="42">
+      <c r="J6" s="43">
         <f>J3/100*J4*J10</f>
         <v>-145.7</v>
       </c>
     </row>
-    <row r="7" s="19" customFormat="1" spans="1:10">
-      <c r="A7" s="27" t="s">
+    <row r="7" s="20" customFormat="1" spans="1:10">
+      <c r="A7" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="33">
+      <c r="B7" s="34">
         <v>10</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="35">
         <v>4</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="31">
         <f t="shared" si="0"/>
         <v>196.025329071332</v>
       </c>
-      <c r="F7" s="35">
+      <c r="F7" s="36">
         <f>IF($B$1="BUY",F6*(1-$B$5/100),F6*(1+$B$5/100))</f>
         <v>1.58965405098421</v>
       </c>
-      <c r="G7" s="32">
+      <c r="G7" s="33">
         <f t="shared" si="1"/>
         <v>311.612458453756</v>
       </c>
-      <c r="I7" s="27" t="s">
+      <c r="I7" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="J7" s="33">
+      <c r="J7" s="34">
         <f>IF(B1="BUY",(((J10/F3)-1)*-1),(J10/F3)-1)*100</f>
         <v>15.1400952418302</v>
       </c>
     </row>
-    <row r="8" s="19" customFormat="1" spans="1:7">
-      <c r="A8" s="27" t="s">
+    <row r="8" s="20" customFormat="1" spans="1:7">
+      <c r="A8" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="33">
+      <c r="B8" s="34">
         <f>B3*$B$9/100</f>
         <v>101.99</v>
       </c>
-      <c r="D8" s="34">
+      <c r="D8" s="35">
         <v>5</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="31">
         <f t="shared" si="0"/>
         <v>254.832927792732</v>
       </c>
-      <c r="F8" s="35">
+      <c r="F8" s="36">
         <f>IF($B$1="BUY",F7*(1-$B$5/100),F7*(1+$B$5/100))</f>
         <v>1.61667816985094</v>
       </c>
-      <c r="G8" s="32">
+      <c r="G8" s="33">
         <f t="shared" si="1"/>
         <v>411.982831321711</v>
       </c>
     </row>
-    <row r="9" s="19" customFormat="1" spans="1:10">
-      <c r="A9" s="27" t="s">
+    <row r="9" s="20" customFormat="1" spans="1:10">
+      <c r="A9" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="28">
+      <c r="B9" s="29">
         <v>7</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="35">
         <v>6</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="31">
         <f t="shared" si="0"/>
         <v>331.282806130552</v>
       </c>
-      <c r="F9" s="35">
+      <c r="F9" s="36">
         <f>IF($B$1="BUY",F8*(1-$B$5/100),F8*(1+$B$5/100))</f>
         <v>1.6441616987384</v>
       </c>
-      <c r="G9" s="32">
+      <c r="G9" s="33">
         <f t="shared" si="1"/>
         <v>544.682501290432</v>
       </c>
-      <c r="I9" s="27" t="s">
+      <c r="I9" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="J9" s="27" t="s">
+      <c r="J9" s="28" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" s="19" customFormat="1" ht="17.4" spans="1:10">
-      <c r="A10" s="27" t="s">
+    <row r="10" s="20" customFormat="1" ht="17.4" spans="1:10">
+      <c r="A10" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="33">
+      <c r="B10" s="34">
         <v>10</v>
       </c>
-      <c r="D10" s="34">
+      <c r="D10" s="35">
         <v>7</v>
       </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="32">
+      <c r="E10" s="31"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I10" s="43">
+      <c r="I10" s="44">
         <f>G18/E18</f>
         <v>1.59024720907573</v>
       </c>
-      <c r="J10" s="44">
+      <c r="J10" s="45">
         <f>IF(B1="BUY",((B4/G18)+1)*I10,((B4/-G18)+1)*I10)</f>
         <v>1.7109818152936</v>
       </c>
     </row>
-    <row r="11" s="19" customFormat="1" spans="4:7">
-      <c r="D11" s="34">
+    <row r="11" s="20" customFormat="1" spans="4:7">
+      <c r="D11" s="35">
         <v>8</v>
       </c>
-      <c r="E11" s="30"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="32">
+      <c r="E11" s="31"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" s="19" customFormat="1" spans="4:7">
-      <c r="D12" s="34">
+    <row r="12" s="20" customFormat="1" spans="4:7">
+      <c r="D12" s="35">
         <v>9</v>
       </c>
-      <c r="E12" s="30"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="32">
+      <c r="E12" s="31"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" s="19" customFormat="1" spans="4:10">
-      <c r="D13" s="34">
+    <row r="13" s="20" customFormat="1" spans="4:10">
+      <c r="D13" s="35">
         <v>10</v>
       </c>
-      <c r="E13" s="30"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="32">
+      <c r="E13" s="31"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I13" s="45" t="s">
+      <c r="I13" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="J13" s="45"/>
-    </row>
-    <row r="14" s="19" customFormat="1" spans="4:9">
-      <c r="D14" s="34">
+      <c r="J13" s="46"/>
+    </row>
+    <row r="14" s="20" customFormat="1" spans="4:9">
+      <c r="D14" s="35">
         <v>11</v>
       </c>
-      <c r="E14" s="30"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="32"/>
-      <c r="I14" s="46" t="s">
+      <c r="E14" s="31"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="33"/>
+      <c r="I14" s="47" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" s="19" customFormat="1" spans="4:9">
-      <c r="D15" s="34">
+    <row r="15" s="20" customFormat="1" spans="4:9">
+      <c r="D15" s="35">
         <v>12</v>
       </c>
-      <c r="E15" s="30"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="32"/>
-      <c r="I15" s="33">
+      <c r="E15" s="31"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="33"/>
+      <c r="I15" s="34">
         <f>IF(B1="BUY",F3*(1-(J7)/100),F3*(1+(J7)/100))</f>
         <v>1.7109818152936</v>
       </c>
     </row>
-    <row r="16" s="19" customFormat="1" spans="4:9">
-      <c r="D16" s="34">
+    <row r="16" s="20" customFormat="1" spans="4:9">
+      <c r="D16" s="35">
         <v>13</v>
       </c>
-      <c r="E16" s="30"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="32"/>
-      <c r="I16" s="47" t="s">
+      <c r="E16" s="31"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="33"/>
+      <c r="I16" s="48" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" s="19" customFormat="1" ht="18.15" spans="3:10">
-      <c r="C17" s="19" t="s">
+    <row r="17" s="20" customFormat="1" ht="18.15" spans="3:10">
+      <c r="C17" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="37" t="s">
+      <c r="D17" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="38"/>
-      <c r="F17" s="39">
+      <c r="E17" s="39"/>
+      <c r="F17" s="40">
         <f>IF(B1="BUY",MIN(F3:F16)*(1-($B$5/3)/100),MAX(F3:F16)*(1+($B$5/3)/100))</f>
         <v>1.65347861503125</v>
       </c>
-      <c r="G17" s="40">
+      <c r="G17" s="41">
         <f>E17*F17</f>
         <v>0</v>
       </c>
-      <c r="I17" s="33">
+      <c r="I17" s="34">
         <f>IF(B1="BUY",(((I15/I10)-1)*-1),((I15/I10)-1))*100</f>
         <v>7.59219104607256</v>
       </c>
-      <c r="J17" s="43" t="str">
+      <c r="J17" s="44" t="str">
         <f>IF(B1="BUY","TIENE QUE SUBIR","TIENE QUE BAJAR")</f>
         <v>TIENE QUE BAJAR</v>
       </c>
     </row>
-    <row r="18" s="19" customFormat="1" spans="4:9">
-      <c r="D18" s="41"/>
-      <c r="E18" s="41">
+    <row r="18" s="20" customFormat="1" spans="4:9">
+      <c r="D18" s="42"/>
+      <c r="E18" s="42">
         <f>SUM(E3:E17)</f>
         <v>1206.77910471736</v>
       </c>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41">
+      <c r="F18" s="42"/>
+      <c r="G18" s="42">
         <f>SUM(G3:G17)</f>
         <v>1919.07710324769</v>
       </c>
-      <c r="H18" s="41"/>
-      <c r="I18" s="47" t="s">
+      <c r="H18" s="42"/>
+      <c r="I18" s="48" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" s="19" customFormat="1" spans="9:9">
-      <c r="I19" s="48">
+    <row r="19" s="20" customFormat="1" spans="9:9">
+      <c r="I19" s="49">
         <f>G18/B3</f>
         <v>1.31714282995724</v>
       </c>
     </row>
-    <row r="20" s="19" customFormat="1"/>
-    <row r="21" s="19" customFormat="1"/>
-    <row r="22" s="19" customFormat="1" spans="16376:16384">
-      <c r="XEV22" s="20"/>
-      <c r="XEW22" s="20"/>
-      <c r="XEX22" s="20"/>
-      <c r="XEY22" s="20"/>
-      <c r="XEZ22" s="20"/>
-      <c r="XFA22" s="20"/>
-      <c r="XFB22" s="20"/>
-      <c r="XFC22" s="20"/>
-      <c r="XFD22" s="20"/>
-    </row>
-    <row r="23" s="19" customFormat="1" spans="16376:16384">
-      <c r="XEV23" s="20"/>
-      <c r="XEW23" s="20"/>
-      <c r="XEX23" s="20"/>
-      <c r="XEY23" s="20"/>
-      <c r="XEZ23" s="20"/>
-      <c r="XFA23" s="20"/>
-      <c r="XFB23" s="20"/>
-      <c r="XFC23" s="20"/>
-      <c r="XFD23" s="20"/>
-    </row>
-    <row r="24" s="19" customFormat="1" spans="16376:16384">
-      <c r="XEV24" s="20"/>
-      <c r="XEW24" s="20"/>
-      <c r="XEX24" s="20"/>
-      <c r="XEY24" s="20"/>
-      <c r="XEZ24" s="20"/>
-      <c r="XFA24" s="20"/>
-      <c r="XFB24" s="20"/>
-      <c r="XFC24" s="20"/>
-      <c r="XFD24" s="20"/>
+    <row r="20" s="20" customFormat="1"/>
+    <row r="21" s="20" customFormat="1"/>
+    <row r="22" s="20" customFormat="1" spans="16376:16384">
+      <c r="XEV22" s="21"/>
+      <c r="XEW22" s="21"/>
+      <c r="XEX22" s="21"/>
+      <c r="XEY22" s="21"/>
+      <c r="XEZ22" s="21"/>
+      <c r="XFA22" s="21"/>
+      <c r="XFB22" s="21"/>
+      <c r="XFC22" s="21"/>
+      <c r="XFD22" s="21"/>
+    </row>
+    <row r="23" s="20" customFormat="1" spans="16376:16384">
+      <c r="XEV23" s="21"/>
+      <c r="XEW23" s="21"/>
+      <c r="XEX23" s="21"/>
+      <c r="XEY23" s="21"/>
+      <c r="XEZ23" s="21"/>
+      <c r="XFA23" s="21"/>
+      <c r="XFB23" s="21"/>
+      <c r="XFC23" s="21"/>
+      <c r="XFD23" s="21"/>
+    </row>
+    <row r="24" s="20" customFormat="1" spans="16376:16384">
+      <c r="XEV24" s="21"/>
+      <c r="XEW24" s="21"/>
+      <c r="XEX24" s="21"/>
+      <c r="XEY24" s="21"/>
+      <c r="XEZ24" s="21"/>
+      <c r="XFA24" s="21"/>
+      <c r="XFB24" s="21"/>
+      <c r="XFC24" s="21"/>
+      <c r="XFD24" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2443,447 +2514,441 @@
   <sheetPr/>
   <dimension ref="A1:XFD24"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44444444444444" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22" style="19" customWidth="1"/>
-    <col min="2" max="2" width="12.8888888888889" style="19" customWidth="1"/>
-    <col min="3" max="3" width="4.55555555555556" style="19" customWidth="1"/>
-    <col min="4" max="4" width="8.44444444444444" style="19" customWidth="1"/>
-    <col min="5" max="5" width="18.5555555555556" style="19" customWidth="1"/>
-    <col min="6" max="6" width="17.1111111111111" style="19" customWidth="1"/>
-    <col min="7" max="7" width="15.6666666666667" style="19" customWidth="1"/>
-    <col min="8" max="8" width="1.66666666666667" style="19" customWidth="1"/>
-    <col min="9" max="9" width="32.8888888888889" style="19" customWidth="1"/>
-    <col min="10" max="10" width="31.2222222222222" style="19" customWidth="1"/>
-    <col min="11" max="11" width="8.44444444444444" style="19" customWidth="1"/>
-    <col min="12" max="12" width="31.2222222222222" style="19" customWidth="1"/>
-    <col min="13" max="16374" width="8.44444444444444" style="19" customWidth="1"/>
-    <col min="16375" max="16375" width="8.44444444444444" style="19"/>
-    <col min="16376" max="16384" width="8.44444444444444" style="20"/>
+    <col min="1" max="1" width="22" style="20" customWidth="1"/>
+    <col min="2" max="2" width="12.8888888888889" style="20" customWidth="1"/>
+    <col min="3" max="3" width="4.55555555555556" style="20" customWidth="1"/>
+    <col min="4" max="4" width="8.44444444444444" style="20" customWidth="1"/>
+    <col min="5" max="5" width="18.5555555555556" style="20" customWidth="1"/>
+    <col min="6" max="6" width="17.1111111111111" style="20" customWidth="1"/>
+    <col min="7" max="7" width="15.6666666666667" style="20" customWidth="1"/>
+    <col min="8" max="8" width="1.66666666666667" style="20" customWidth="1"/>
+    <col min="9" max="9" width="32.8888888888889" style="20" customWidth="1"/>
+    <col min="10" max="10" width="31.2222222222222" style="20" customWidth="1"/>
+    <col min="11" max="11" width="8.44444444444444" style="20" customWidth="1"/>
+    <col min="12" max="12" width="31.2222222222222" style="20" customWidth="1"/>
+    <col min="13" max="16374" width="8.44444444444444" style="20" customWidth="1"/>
+    <col min="16375" max="16375" width="8.44444444444444" style="20"/>
+    <col min="16376" max="16384" width="8.44444444444444" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" s="19" customFormat="1" ht="15.75" spans="1:2">
-      <c r="A1" s="21" t="s">
+    <row r="1" s="20" customFormat="1" ht="15.75" spans="1:2">
+      <c r="A1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="23" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" s="19" customFormat="1" ht="15.15" spans="4:7">
-      <c r="D2" s="23" t="s">
+    <row r="2" s="20" customFormat="1" ht="15.15" spans="4:7">
+      <c r="D2" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="27" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" s="19" customFormat="1" spans="1:10">
-      <c r="A3" s="27" t="s">
+    <row r="3" s="20" customFormat="1" spans="1:10">
+      <c r="A3" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="28">
-        <v>1457</v>
-      </c>
-      <c r="D3" s="29" t="s">
+      <c r="B3" s="29">
+        <v>1516</v>
+      </c>
+      <c r="D3" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="30">
+      <c r="E3" s="31">
         <f>G3/F3</f>
-        <v>41.6682554814109</v>
-      </c>
-      <c r="F3" s="31">
+        <v>72.2592945662536</v>
+      </c>
+      <c r="F3" s="32">
         <v>2.098</v>
       </c>
-      <c r="G3" s="32">
+      <c r="G3" s="33">
         <f>B8</f>
-        <v>87.42</v>
-      </c>
-      <c r="I3" s="27" t="s">
+        <v>151.6</v>
+      </c>
+      <c r="I3" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="42">
+      <c r="J3" s="43">
         <f>IF(B1="BUY",((I10/J10)-1)*-100,((I10/J10)-1)*100)</f>
-        <v>-4.51931637716719</v>
-      </c>
-    </row>
-    <row r="4" s="19" customFormat="1" spans="1:10">
-      <c r="A4" s="27" t="s">
+        <v>-6.2746342102956</v>
+      </c>
+    </row>
+    <row r="4" s="20" customFormat="1" spans="1:10">
+      <c r="A4" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="33">
+      <c r="B4" s="34">
         <f>-B3*$B$10/100</f>
-        <v>-145.7</v>
-      </c>
-      <c r="D4" s="34">
+        <v>-151.6</v>
+      </c>
+      <c r="D4" s="35">
         <v>1</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="31">
         <f t="shared" ref="E4:E11" si="0">E3*(1+$B$6/100)</f>
-        <v>54.1687321258341</v>
-      </c>
-      <c r="F4" s="35">
+        <v>83.0981887511916</v>
+      </c>
+      <c r="F4" s="36">
         <f>IF($B$1="BUY",F3*(1-$B$5/100),F3*(1+$B$5/100))</f>
-        <v>2.133666</v>
-      </c>
-      <c r="G4" s="32">
+        <v>2.13996</v>
+      </c>
+      <c r="G4" s="33">
         <f t="shared" ref="G4:G17" si="1">E4*F4</f>
-        <v>115.577982</v>
-      </c>
-      <c r="I4" s="27" t="s">
+        <v>177.8268</v>
+      </c>
+      <c r="I4" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="42">
+      <c r="J4" s="43">
         <f>E18</f>
-        <v>1334.00911215072</v>
-      </c>
-    </row>
-    <row r="5" s="19" customFormat="1" spans="1:10">
-      <c r="A5" s="27" t="s">
+        <v>991.890263619071</v>
+      </c>
+    </row>
+    <row r="5" s="20" customFormat="1" spans="1:10">
+      <c r="A5" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="34">
+      <c r="D5" s="35">
         <v>2</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="31">
         <f t="shared" si="0"/>
-        <v>70.4193517635844</v>
-      </c>
-      <c r="F5" s="35">
+        <v>95.5629170638703</v>
+      </c>
+      <c r="F5" s="36">
         <f>IF($B$1="BUY",F4*(1-$B$5/100),F4*(1+$B$5/100))</f>
-        <v>2.169938322</v>
-      </c>
-      <c r="G5" s="32">
+        <v>2.1827592</v>
+      </c>
+      <c r="G5" s="33">
         <f t="shared" si="1"/>
-        <v>152.8056500022</v>
-      </c>
-      <c r="I5" s="27" t="s">
+        <v>208.5908364</v>
+      </c>
+      <c r="I5" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="42">
+      <c r="J5" s="43">
         <f>J4*J10</f>
-        <v>3223.93892881932</v>
-      </c>
-    </row>
-    <row r="6" s="19" customFormat="1" spans="1:10">
-      <c r="A6" s="27" t="s">
+        <v>2416.07709579708</v>
+      </c>
+    </row>
+    <row r="6" s="20" customFormat="1" spans="1:10">
+      <c r="A6" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="33">
+      <c r="B6" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="35">
+        <v>3</v>
+      </c>
+      <c r="E6" s="31">
+        <f t="shared" si="0"/>
+        <v>109.897354623451</v>
+      </c>
+      <c r="F6" s="36">
+        <f>IF($B$1="BUY",F5*(1-$B$5/100),F5*(1+$B$5/100))</f>
+        <v>2.226414384</v>
+      </c>
+      <c r="G6" s="33">
+        <f t="shared" si="1"/>
+        <v>244.6770510972</v>
+      </c>
+      <c r="I6" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="43">
+        <f>J3/100*J4*J10</f>
+        <v>-151.6</v>
+      </c>
+    </row>
+    <row r="7" s="20" customFormat="1" spans="1:10">
+      <c r="A7" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="34">
+        <v>10</v>
+      </c>
+      <c r="D7" s="35">
+        <v>4</v>
+      </c>
+      <c r="E7" s="31">
+        <f t="shared" si="0"/>
+        <v>126.381957816968</v>
+      </c>
+      <c r="F7" s="36">
+        <f>IF($B$1="BUY",F6*(1-$B$5/100),F6*(1+$B$5/100))</f>
+        <v>2.27094267168</v>
+      </c>
+      <c r="G7" s="33">
+        <f t="shared" si="1"/>
+        <v>287.006180937015</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="34">
+        <f>IF(B1="BUY",(((J10/F3)-1)*-1),(J10/F3)-1)*100</f>
+        <v>16.1025282854034</v>
+      </c>
+    </row>
+    <row r="8" s="20" customFormat="1" spans="1:7">
+      <c r="A8" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="34">
+        <f>B3*$B$9/100</f>
+        <v>151.6</v>
+      </c>
+      <c r="D8" s="35">
+        <v>5</v>
+      </c>
+      <c r="E8" s="31">
+        <f t="shared" si="0"/>
+        <v>145.339251489514</v>
+      </c>
+      <c r="F8" s="36">
+        <f>IF($B$1="BUY",F7*(1-$B$5/100),F7*(1+$B$5/100))</f>
+        <v>2.3163615251136</v>
+      </c>
+      <c r="G8" s="33">
+        <f t="shared" si="1"/>
+        <v>336.658250239119</v>
+      </c>
+    </row>
+    <row r="9" s="20" customFormat="1" spans="1:10">
+      <c r="A9" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="29">
+        <v>10</v>
+      </c>
+      <c r="D9" s="35">
+        <v>6</v>
+      </c>
+      <c r="E9" s="31">
+        <f>E8*(1+$B$6/100)</f>
+        <v>167.140139212941</v>
+      </c>
+      <c r="F9" s="36">
+        <f>IF($B$1="BUY",F8*(1-$B$5/100),F8*(1+$B$5/100))</f>
+        <v>2.36268875561587</v>
+      </c>
+      <c r="G9" s="33">
+        <f t="shared" si="1"/>
+        <v>394.900127530487</v>
+      </c>
+      <c r="I9" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="34">
-        <v>3</v>
-      </c>
-      <c r="E6" s="30">
-        <f t="shared" si="0"/>
-        <v>91.5451572926597</v>
-      </c>
-      <c r="F6" s="35">
-        <f>IF($B$1="BUY",F5*(1-$B$5/100),F5*(1+$B$5/100))</f>
-        <v>2.206827273474</v>
-      </c>
-      <c r="G6" s="32">
-        <f t="shared" si="1"/>
-        <v>202.024349867909</v>
-      </c>
-      <c r="I6" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6" s="42">
-        <f>J3/100*J4*J10</f>
-        <v>-145.7</v>
-      </c>
-    </row>
-    <row r="7" s="19" customFormat="1" spans="1:10">
-      <c r="A7" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="33">
+      <c r="J9" s="28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" s="20" customFormat="1" ht="17.4" spans="1:10">
+      <c r="A10" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="34">
         <v>10</v>
       </c>
-      <c r="D7" s="34">
-        <v>4</v>
-      </c>
-      <c r="E7" s="30">
-        <f t="shared" si="0"/>
-        <v>119.008704480458</v>
-      </c>
-      <c r="F7" s="35">
-        <f>IF($B$1="BUY",F6*(1-$B$5/100),F6*(1+$B$5/100))</f>
-        <v>2.24434333712306</v>
-      </c>
-      <c r="G7" s="32">
-        <f t="shared" si="1"/>
-        <v>267.096392960362</v>
-      </c>
-      <c r="I7" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="J7" s="33">
-        <f>IF(B1="BUY",(((J10/F3)-1)*-1),(J10/F3)-1)*100</f>
-        <v>15.1920550884314</v>
-      </c>
-    </row>
-    <row r="8" s="19" customFormat="1" spans="1:7">
-      <c r="A8" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="33">
-        <f>B3*$B$9/100</f>
-        <v>87.42</v>
-      </c>
-      <c r="D8" s="34">
-        <v>5</v>
-      </c>
-      <c r="E8" s="30">
-        <f t="shared" si="0"/>
-        <v>154.711315824595</v>
-      </c>
-      <c r="F8" s="35">
-        <f>IF($B$1="BUY",F7*(1-$B$5/100),F7*(1+$B$5/100))</f>
-        <v>2.28249717385415</v>
-      </c>
-      <c r="G8" s="32">
-        <f t="shared" si="1"/>
-        <v>353.128141132895</v>
-      </c>
-    </row>
-    <row r="9" s="19" customFormat="1" spans="1:10">
-      <c r="A9" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="28">
-        <v>6</v>
-      </c>
-      <c r="D9" s="34">
-        <v>6</v>
-      </c>
-      <c r="E9" s="30">
-        <f t="shared" si="0"/>
-        <v>201.124710571973</v>
-      </c>
-      <c r="F9" s="35">
-        <f>IF($B$1="BUY",F8*(1-$B$5/100),F8*(1+$B$5/100))</f>
-        <v>2.32129962580967</v>
-      </c>
-      <c r="G9" s="32">
-        <f t="shared" si="1"/>
-        <v>466.8707153918</v>
-      </c>
-      <c r="I9" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="J9" s="27" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" s="19" customFormat="1" ht="17.4" spans="1:10">
-      <c r="A10" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="33">
-        <v>10</v>
-      </c>
-      <c r="D10" s="34">
+      <c r="D10" s="35">
         <v>7</v>
       </c>
-      <c r="E10" s="30">
-        <f t="shared" si="0"/>
-        <v>261.462123743565</v>
-      </c>
-      <c r="F10" s="35">
+      <c r="E10" s="31">
+        <f>E9*(1+$B$6/100)</f>
+        <v>192.211160094882</v>
+      </c>
+      <c r="F10" s="36">
         <f>IF($B$1="BUY",F9*(1-$B$5/100),F9*(1+$B$5/100))</f>
-        <v>2.36076171944843</v>
-      </c>
-      <c r="G10" s="32">
+        <v>2.40994253072819</v>
+      </c>
+      <c r="G10" s="33">
         <f t="shared" ref="G10:G16" si="2">E10*F10</f>
-        <v>617.249772819499</v>
-      </c>
-      <c r="I10" s="43">
+        <v>463.217849593261</v>
+      </c>
+      <c r="I10" s="44">
         <f>G18/E18</f>
-        <v>2.30750967199656</v>
-      </c>
-      <c r="J10" s="44">
+        <v>2.28299155547184</v>
+      </c>
+      <c r="J10" s="45">
         <f>IF(B1="BUY",((B4/G18)+1)*I10,((B4/-G18)+1)*I10)</f>
-        <v>2.41672931575529</v>
-      </c>
-    </row>
-    <row r="11" s="19" customFormat="1" spans="1:7">
-      <c r="A11" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="36">
+        <v>2.43583104342776</v>
+      </c>
+    </row>
+    <row r="11" s="20" customFormat="1" spans="1:7">
+      <c r="A11" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="37">
         <f>B8*0.7/100</f>
-        <v>0.61194</v>
-      </c>
-      <c r="D11" s="34">
+        <v>1.0612</v>
+      </c>
+      <c r="D11" s="35">
         <v>8</v>
       </c>
-      <c r="E11" s="30">
-        <f t="shared" si="0"/>
-        <v>339.900760866635</v>
-      </c>
-      <c r="F11" s="35">
-        <f>IF($B$1="BUY",F10*(1-$B$5/100),F10*(1+$B$5/100))</f>
-        <v>2.40089466867906</v>
-      </c>
-      <c r="G11" s="32">
-        <f t="shared" si="2"/>
-        <v>816.065924644659</v>
-      </c>
-    </row>
-    <row r="12" s="19" customFormat="1" spans="4:7">
-      <c r="D12" s="34">
-        <v>9</v>
-      </c>
-      <c r="E12" s="30"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="32">
+      <c r="E11" s="31"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="33">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" s="19" customFormat="1" spans="4:10">
-      <c r="D13" s="34">
-        <v>10</v>
-      </c>
-      <c r="E13" s="30"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="32">
+    <row r="12" s="20" customFormat="1" spans="4:7">
+      <c r="D12" s="35">
+        <v>9</v>
+      </c>
+      <c r="E12" s="31"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="33">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I13" s="45" t="s">
+    </row>
+    <row r="13" s="20" customFormat="1" spans="4:10">
+      <c r="D13" s="35">
+        <v>10</v>
+      </c>
+      <c r="E13" s="31"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="J13" s="45"/>
-    </row>
-    <row r="14" s="19" customFormat="1" spans="4:9">
-      <c r="D14" s="34">
+      <c r="J13" s="46"/>
+    </row>
+    <row r="14" s="20" customFormat="1" spans="4:9">
+      <c r="D14" s="35">
         <v>11</v>
       </c>
-      <c r="E14" s="30"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="32"/>
-      <c r="I14" s="46" t="s">
+      <c r="E14" s="31"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="33"/>
+      <c r="I14" s="47" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" s="19" customFormat="1" spans="4:9">
-      <c r="D15" s="34">
+    <row r="15" s="20" customFormat="1" spans="4:9">
+      <c r="D15" s="35">
         <v>12</v>
       </c>
-      <c r="E15" s="30"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="32"/>
-      <c r="I15" s="33">
+      <c r="E15" s="31"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="33"/>
+      <c r="I15" s="34">
         <f>IF(B1="BUY",F3*(1-(J7)/100),F3*(1+(J7)/100))</f>
-        <v>2.41672931575529</v>
-      </c>
-    </row>
-    <row r="16" s="19" customFormat="1" spans="4:9">
-      <c r="D16" s="34">
+        <v>2.43583104342776</v>
+      </c>
+    </row>
+    <row r="16" s="20" customFormat="1" spans="4:9">
+      <c r="D16" s="35">
         <v>13</v>
       </c>
-      <c r="E16" s="30"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="32"/>
-      <c r="I16" s="47" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" s="19" customFormat="1" ht="18.15" spans="4:10">
-      <c r="D17" s="37" t="s">
+      <c r="E16" s="31"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="33"/>
+      <c r="I16" s="48" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" s="20" customFormat="1" ht="18.15" spans="4:10">
+      <c r="D17" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="38"/>
-      <c r="F17" s="39">
+      <c r="E17" s="39"/>
+      <c r="F17" s="40">
         <f>IF(B1="BUY",MIN(F3:F16)*(1-($B$5/3)/100),MAX(F3:F16)*(1+($B$5/3)/100))</f>
-        <v>2.41449973846824</v>
-      </c>
-      <c r="G17" s="40">
+        <v>2.42600881426638</v>
+      </c>
+      <c r="G17" s="41">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I17" s="33">
+      <c r="I17" s="34">
         <f>IF(B1="BUY",(((I15/I10)-1)*-1),((I15/I10)-1))*100</f>
-        <v>4.73322582714151</v>
-      </c>
-      <c r="J17" s="43" t="str">
+        <v>6.69470229049227</v>
+      </c>
+      <c r="J17" s="44" t="str">
         <f>IF(B1="BUY","TIENE QUE SUBIR","TIENE QUE BAJAR")</f>
         <v>TIENE QUE BAJAR</v>
       </c>
     </row>
-    <row r="18" s="19" customFormat="1" spans="4:9">
-      <c r="D18" s="41"/>
-      <c r="E18" s="41">
+    <row r="18" s="20" customFormat="1" spans="4:9">
+      <c r="D18" s="42"/>
+      <c r="E18" s="42">
         <f>SUM(E3:E17)</f>
-        <v>1334.00911215072</v>
-      </c>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41">
+        <v>991.890263619071</v>
+      </c>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42">
         <f>SUM(G3:G17)</f>
-        <v>3078.23892881932</v>
-      </c>
-      <c r="H18" s="41"/>
-      <c r="I18" s="47" t="s">
+        <v>2264.47709579708</v>
+      </c>
+      <c r="H18" s="42"/>
+      <c r="I18" s="48" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" s="19" customFormat="1" spans="9:9">
-      <c r="I19" s="48">
+    <row r="19" s="20" customFormat="1" spans="9:9">
+      <c r="I19" s="49">
         <f>G18/B3</f>
-        <v>2.11272404174284</v>
-      </c>
-    </row>
-    <row r="20" s="19" customFormat="1"/>
-    <row r="21" s="19" customFormat="1"/>
-    <row r="22" s="19" customFormat="1" spans="16376:16384">
-      <c r="XEV22" s="20"/>
-      <c r="XEW22" s="20"/>
-      <c r="XEX22" s="20"/>
-      <c r="XEY22" s="20"/>
-      <c r="XEZ22" s="20"/>
-      <c r="XFA22" s="20"/>
-      <c r="XFB22" s="20"/>
-      <c r="XFC22" s="20"/>
-      <c r="XFD22" s="20"/>
-    </row>
-    <row r="23" s="19" customFormat="1" spans="16376:16384">
-      <c r="XEV23" s="20"/>
-      <c r="XEW23" s="20"/>
-      <c r="XEX23" s="20"/>
-      <c r="XEY23" s="20"/>
-      <c r="XEZ23" s="20"/>
-      <c r="XFA23" s="20"/>
-      <c r="XFB23" s="20"/>
-      <c r="XFC23" s="20"/>
-      <c r="XFD23" s="20"/>
-    </row>
-    <row r="24" s="19" customFormat="1" spans="16376:16384">
-      <c r="XEV24" s="20"/>
-      <c r="XEW24" s="20"/>
-      <c r="XEX24" s="20"/>
-      <c r="XEY24" s="20"/>
-      <c r="XEZ24" s="20"/>
-      <c r="XFA24" s="20"/>
-      <c r="XFB24" s="20"/>
-      <c r="XFC24" s="20"/>
-      <c r="XFD24" s="20"/>
+        <v>1.49371840092156</v>
+      </c>
+    </row>
+    <row r="20" s="20" customFormat="1"/>
+    <row r="21" s="20" customFormat="1"/>
+    <row r="22" s="20" customFormat="1" spans="16376:16384">
+      <c r="XEV22" s="21"/>
+      <c r="XEW22" s="21"/>
+      <c r="XEX22" s="21"/>
+      <c r="XEY22" s="21"/>
+      <c r="XEZ22" s="21"/>
+      <c r="XFA22" s="21"/>
+      <c r="XFB22" s="21"/>
+      <c r="XFC22" s="21"/>
+      <c r="XFD22" s="21"/>
+    </row>
+    <row r="23" s="20" customFormat="1" spans="16376:16384">
+      <c r="XEV23" s="21"/>
+      <c r="XEW23" s="21"/>
+      <c r="XEX23" s="21"/>
+      <c r="XEY23" s="21"/>
+      <c r="XEZ23" s="21"/>
+      <c r="XFA23" s="21"/>
+      <c r="XFB23" s="21"/>
+      <c r="XFC23" s="21"/>
+      <c r="XFD23" s="21"/>
+    </row>
+    <row r="24" s="20" customFormat="1" spans="16376:16384">
+      <c r="XEV24" s="21"/>
+      <c r="XEW24" s="21"/>
+      <c r="XEX24" s="21"/>
+      <c r="XEY24" s="21"/>
+      <c r="XEZ24" s="21"/>
+      <c r="XFA24" s="21"/>
+      <c r="XFB24" s="21"/>
+      <c r="XFC24" s="21"/>
+      <c r="XFD24" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2967,210 +3032,210 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13" style="6" customWidth="1"/>
-    <col min="2" max="2" width="11.4444444444444" style="6" customWidth="1"/>
-    <col min="3" max="3" width="8.88888888888889" style="6"/>
-    <col min="4" max="4" width="9" style="6" customWidth="1"/>
-    <col min="5" max="5" width="12.5555555555556" style="6" customWidth="1"/>
-    <col min="6" max="6" width="11.1111111111111" style="6" customWidth="1"/>
-    <col min="7" max="7" width="10.2222222222222" style="6" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="12" style="6" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="11" style="6" customWidth="1"/>
-    <col min="10" max="10" width="10.2222222222222" style="6" customWidth="1"/>
-    <col min="11" max="11" width="14.7777777777778" style="6" customWidth="1"/>
-    <col min="12" max="16384" width="8.88888888888889" style="6"/>
+    <col min="1" max="1" width="13" style="7" customWidth="1"/>
+    <col min="2" max="2" width="11.4444444444444" style="7" customWidth="1"/>
+    <col min="3" max="3" width="8.88888888888889" style="7"/>
+    <col min="4" max="4" width="9" style="7" customWidth="1"/>
+    <col min="5" max="5" width="12.5555555555556" style="7" customWidth="1"/>
+    <col min="6" max="6" width="11.1111111111111" style="7" customWidth="1"/>
+    <col min="7" max="7" width="10.2222222222222" style="7" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="12" style="7" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="7" customWidth="1"/>
+    <col min="10" max="10" width="10.2222222222222" style="7" customWidth="1"/>
+    <col min="11" max="11" width="14.7777777777778" style="7" customWidth="1"/>
+    <col min="12" max="16384" width="8.88888888888889" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
+      <c r="A1" s="8"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="9" t="s">
+      <c r="A2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="F2" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="G2" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="H2" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="I2" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="J2" s="10" t="s">
         <v>49</v>
       </c>
+      <c r="K2" s="10" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="12">
         <v>112</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" s="11">
+      <c r="C3" s="8"/>
+      <c r="D3" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="12">
         <v>109.75</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="12">
         <v>13.202</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="14">
         <f t="shared" ref="G3:G6" si="0">E3/F3</f>
         <v>8.31313437357976</v>
       </c>
-      <c r="H3" s="14">
+      <c r="H3" s="15">
         <f>IF(A2="BUY",((I3/J3)-1)*-100,((I3/J3)-1)*100)</f>
         <v>-11.3647894469812</v>
       </c>
-      <c r="I3" s="14">
+      <c r="I3" s="15">
         <f>SUM(E3:E4)/SUM(G3:G4)</f>
         <v>13.202</v>
       </c>
-      <c r="J3" s="14">
+      <c r="J3" s="15">
         <f>IF(A2="BUY",((B5/SUM(E3:E4))+1)*I3,((B5/-SUM(E3:E4))+1)*I3)</f>
         <v>11.8547343963554</v>
       </c>
-      <c r="K3" s="16">
+      <c r="K3" s="17">
         <f>H3/100*SUM(G3:G4)*J3</f>
         <v>-11.2</v>
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="6">
+      <c r="A4" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="7">
         <v>10</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="E4" s="11">
+      <c r="C4" s="8"/>
+      <c r="D4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="12">
         <v>0</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="12">
         <v>2.2</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="17"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="18"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="14">
         <f>-B3*B4/100</f>
         <v>-11.2</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
     </row>
     <row r="6" spans="3:11">
-      <c r="C6" s="7"/>
-      <c r="D6" s="12" t="s">
+      <c r="C6" s="8"/>
+      <c r="D6" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13">
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14">
         <f>IF(A2="BUY",((F3/J6)-1)*-100,((F3/J6)-1)*100)</f>
         <v>0.692041522491349</v>
       </c>
-      <c r="I6" s="13"/>
-      <c r="J6" s="11">
+      <c r="I6" s="14"/>
+      <c r="J6" s="12">
         <v>13.294</v>
       </c>
-      <c r="K6" s="18">
+      <c r="K6" s="19">
         <f>H6/100*SUM(G3:G4)*J6</f>
         <v>0.764808362369337</v>
       </c>
     </row>
     <row r="7" spans="3:11">
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
     </row>
     <row r="8" spans="3:11">
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
     </row>
     <row r="9" spans="3:10">
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
     </row>
     <row r="10" spans="3:10">
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
     </row>
     <row r="14" spans="5:6">
-      <c r="E14" s="6">
+      <c r="E14" s="7">
         <v>87.36</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="7">
         <f>E14*0.7/100</f>
         <v>0.61152</v>
       </c>
@@ -3218,13 +3283,13 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:E5"/>
+  <dimension ref="B1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="D5:E5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="4"/>
   <cols>
     <col min="2" max="2" width="17.5555555555556" customWidth="1"/>
     <col min="3" max="3" width="12.4444444444444" customWidth="1"/>
@@ -3233,71 +3298,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5">
-      <c r="B1" s="2"/>
-      <c r="C1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>55</v>
       </c>
+      <c r="E1" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="2" spans="2:5">
-      <c r="B2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="3">
         <v>26</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="3">
         <v>2</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="2:5">
-      <c r="B3" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="3">
+      <c r="B3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="4">
         <v>10</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="4">
         <v>6</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="2:5">
-      <c r="B4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="3">
         <v>5</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="3">
         <v>6</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="4">
+      <c r="B5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="5">
         <v>7</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="5">
         <v>6</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="6">
         <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3307,7 +3378,7 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -3324,903 +3395,897 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" hidden="1" spans="1:7">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" hidden="1" spans="1:7">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" t="s">
         <v>70</v>
       </c>
-      <c r="C3" t="s">
-        <v>68</v>
-      </c>
       <c r="D3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" hidden="1" spans="1:7">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" hidden="1" spans="1:7">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" hidden="1" spans="1:7">
+      <c r="A6" t="s">
         <v>68</v>
       </c>
-      <c r="D5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F5" t="s">
-        <v>69</v>
-      </c>
-      <c r="G5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>66</v>
-      </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" hidden="1" spans="1:7">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" hidden="1" spans="1:7">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" t="s">
+        <v>71</v>
+      </c>
+      <c r="G8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
         <v>68</v>
       </c>
-      <c r="D8" t="s">
-        <v>69</v>
-      </c>
-      <c r="E8" t="s">
-        <v>69</v>
-      </c>
-      <c r="F8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" hidden="1" spans="1:7">
-      <c r="A9" t="s">
-        <v>66</v>
-      </c>
       <c r="B9" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C9" t="s">
-        <v>78</v>
-      </c>
-      <c r="D9" t="s">
-        <v>69</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="D9" s="2"/>
       <c r="E9" t="s">
-        <v>69</v>
-      </c>
-      <c r="F9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G9" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="10" hidden="1" spans="1:7">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" hidden="1" spans="1:7">
+      <c r="A11" t="s">
         <v>68</v>
       </c>
-      <c r="D10" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" t="s">
-        <v>69</v>
-      </c>
-      <c r="F10" t="s">
-        <v>69</v>
-      </c>
-      <c r="G10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>66</v>
-      </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D11" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E11" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F11" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G11" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" hidden="1" spans="1:7">
       <c r="A12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B12" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D12" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E12" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F12" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G12" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" hidden="1" spans="1:7">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" hidden="1" spans="1:7">
+      <c r="A14" t="s">
         <v>68</v>
       </c>
-      <c r="D13" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" t="s">
-        <v>69</v>
-      </c>
-      <c r="F13" t="s">
-        <v>69</v>
-      </c>
-      <c r="G13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" t="s">
-        <v>66</v>
-      </c>
       <c r="B14" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D14" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E14" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F14" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G14" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" hidden="1" spans="1:7">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B15" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D15" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E15" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F15" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" hidden="1" spans="1:7">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D16" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E16" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F16" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G16" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" hidden="1" spans="1:4">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B17" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C17" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" hidden="1" spans="1:7">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B18" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D18" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E18" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F18" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" hidden="1" spans="1:7">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B19" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C19" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D19" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E19" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F19" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G19" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" hidden="1" spans="1:7">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B20" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" t="s">
+        <v>71</v>
+      </c>
+      <c r="G20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" hidden="1" spans="1:4">
+      <c r="A21" t="s">
         <v>68</v>
       </c>
-      <c r="D20" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" t="s">
-        <v>69</v>
-      </c>
-      <c r="F20" t="s">
-        <v>69</v>
-      </c>
-      <c r="G20" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>66</v>
-      </c>
       <c r="B21" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C21" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D21" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" hidden="1" spans="1:4">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B22" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C22" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" hidden="1" spans="1:7">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C23" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D23" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E23" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F23" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G23" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" hidden="1" spans="1:7">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B24" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C24" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D24" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E24" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F24" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G24" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" hidden="1" spans="1:7">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B25" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F25" t="s">
+        <v>71</v>
+      </c>
+      <c r="G25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" hidden="1" spans="1:7">
+      <c r="A26" t="s">
         <v>68</v>
       </c>
-      <c r="D25" t="s">
-        <v>69</v>
-      </c>
-      <c r="E25" t="s">
-        <v>69</v>
-      </c>
-      <c r="F25" t="s">
-        <v>69</v>
-      </c>
-      <c r="G25" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" t="s">
-        <v>66</v>
-      </c>
       <c r="B26" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D26" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E26" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F26" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G26" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" hidden="1" spans="1:7">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B27" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C27" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D27" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E27" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F27" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G27" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" hidden="1" spans="1:7">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B28" t="s">
         <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D28" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E28" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F28" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G28" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" hidden="1" spans="1:7">
       <c r="A29" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B29" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C29" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D29" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E29" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F29" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G29" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" hidden="1" spans="1:7">
       <c r="A30" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B30" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C30" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D30" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E30" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F30" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G30" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" hidden="1" spans="1:7">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B31" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C31" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D31" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E31" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F31" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G31" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" hidden="1" spans="1:7">
       <c r="A32" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B32" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C32" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D32" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E32" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F32" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G32" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" hidden="1" spans="1:7">
       <c r="A33" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B33" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C33" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D33" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E33" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F33" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G33" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" hidden="1" spans="1:7">
       <c r="A34" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B34" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C34" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D34" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E34" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F34" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G34" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" hidden="1" spans="1:7">
       <c r="A35" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B35" t="s">
+        <v>108</v>
+      </c>
+      <c r="C35" t="s">
+        <v>70</v>
+      </c>
+      <c r="D35" t="s">
+        <v>71</v>
+      </c>
+      <c r="E35" t="s">
+        <v>71</v>
+      </c>
+      <c r="F35" t="s">
+        <v>71</v>
+      </c>
+      <c r="G35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
         <v>104</v>
       </c>
-      <c r="C35" t="s">
-        <v>68</v>
-      </c>
-      <c r="D35" t="s">
-        <v>69</v>
-      </c>
-      <c r="E35" t="s">
-        <v>69</v>
-      </c>
-      <c r="F35" t="s">
-        <v>69</v>
-      </c>
-      <c r="G35" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="36" hidden="1" spans="1:7">
-      <c r="A36" t="s">
-        <v>100</v>
-      </c>
       <c r="B36" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C36" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D36" t="s">
-        <v>69</v>
-      </c>
-      <c r="E36" t="s">
-        <v>69</v>
-      </c>
-      <c r="F36" t="s">
-        <v>69</v>
-      </c>
-      <c r="G36" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="37" hidden="1" spans="1:7">
       <c r="A37" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B37" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C37" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" hidden="1" spans="1:7">
       <c r="A38" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B38" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C38" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D38" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E38" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F38" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G38" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" hidden="1" spans="1:7">
       <c r="A39" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B39" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="C39" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D39" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E39" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F39" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G39" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" hidden="1" spans="1:7">
       <c r="A40" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B40" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C40" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D40" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E40" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F40" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G40" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G40">
-    <filterColumn colId="2">
-      <customFilters>
-        <customFilter operator="equal" val="POR SELECCION"/>
-      </customFilters>
+    <filterColumn colId="6">
+      <colorFilter dxfId="5"/>
     </filterColumn>
     <extLst/>
   </autoFilter>

</xml_diff>

<commit_message>
nueva estrategia mercado quieto
</commit_message>
<xml_diff>
--- a/SANTA3/FORMULAss.xlsx
+++ b/SANTA3/FORMULAss.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9264" activeTab="2"/>
+    <workbookView windowWidth="22368" windowHeight="9264" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="formula ganancias" sheetId="1" r:id="rId1"/>
@@ -144,7 +144,7 @@
     <t>2</t>
   </si>
   <si>
-    <t>15</t>
+    <t>30</t>
   </si>
   <si>
     <t>primer tp a 0.7 porciento</t>
@@ -204,7 +204,7 @@
     <t>muy movido</t>
   </si>
   <si>
-    <t>buena ganancia:</t>
+    <t>buena ganancia-mercado movido:</t>
   </si>
   <si>
     <t>ARCHIVO</t>
@@ -365,11 +365,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="0.000000"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="0.000000"/>
     <numFmt numFmtId="179" formatCode="0.00000"/>
   </numFmts>
   <fonts count="27">
@@ -437,14 +437,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -461,7 +453,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -476,26 +483,17 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -530,29 +528,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -575,7 +568,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -620,7 +620,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -638,55 +764,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -698,61 +776,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -764,37 +794,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1039,17 +1039,6 @@
       </top>
       <bottom style="medium">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1065,15 +1054,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1117,6 +1097,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1140,18 +1129,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1161,31 +1161,31 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1194,97 +1194,97 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1295,41 +1295,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2496,8 +2496,8 @@
   <sheetPr/>
   <dimension ref="A1:XFD24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:F11"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44444444444444" defaultRowHeight="14.4"/>
@@ -2567,7 +2567,7 @@
       </c>
       <c r="J3" s="42">
         <f>IF(B1="BUY",((I10/J10)-1)*-100,((I10/J10)-1)*100)</f>
-        <v>-7.08250888422096</v>
+        <v>-6.2977081349033</v>
       </c>
     </row>
     <row r="4" s="19" customFormat="1" spans="1:10">
@@ -2598,7 +2598,7 @@
       </c>
       <c r="J4" s="42">
         <f>E18</f>
-        <v>505.72763905901</v>
+        <v>576.524433498759</v>
       </c>
     </row>
     <row r="5" s="19" customFormat="1" spans="1:10">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="E5" s="30">
         <f t="shared" ref="E4:E11" si="1">E4*(1+$B$6/100)</f>
-        <v>48.197270471464</v>
+        <v>54.4838709677419</v>
       </c>
       <c r="F5" s="35">
         <f>IF($B$1="BUY",F4*(1-$B$5/100),F4*(1+$B$5/100))</f>
@@ -2621,14 +2621,14 @@
       </c>
       <c r="G5" s="32">
         <f t="shared" si="0"/>
-        <v>202.082094</v>
+        <v>228.440628</v>
       </c>
       <c r="I5" s="27" t="s">
         <v>23</v>
       </c>
       <c r="J5" s="42">
         <f>J4*J10</f>
-        <v>2384.74815578827</v>
+        <v>2681.92803448477</v>
       </c>
     </row>
     <row r="6" s="19" customFormat="1" spans="1:10">
@@ -2643,7 +2643,7 @@
       </c>
       <c r="E6" s="30">
         <f t="shared" si="1"/>
-        <v>55.4268610421836</v>
+        <v>70.8290322580645</v>
       </c>
       <c r="F6" s="35">
         <f>IF($B$1="BUY",F5*(1-$B$5/100),F5*(1+$B$5/100))</f>
@@ -2651,7 +2651,7 @@
       </c>
       <c r="G6" s="32">
         <f t="shared" si="0"/>
-        <v>237.042296262</v>
+        <v>302.912272728</v>
       </c>
       <c r="I6" s="27" t="s">
         <v>25</v>
@@ -2673,7 +2673,7 @@
       </c>
       <c r="E7" s="30">
         <f t="shared" si="1"/>
-        <v>63.7408901985112</v>
+        <v>92.0777419354839</v>
       </c>
       <c r="F7" s="35">
         <f>IF($B$1="BUY",F6*(1-$B$5/100),F6*(1+$B$5/100))</f>
@@ -2681,14 +2681,14 @@
       </c>
       <c r="G7" s="32">
         <f t="shared" si="0"/>
-        <v>278.050613515326</v>
+        <v>401.661673637328</v>
       </c>
       <c r="I7" s="27" t="s">
         <v>27</v>
       </c>
       <c r="J7" s="33">
         <f>IF(B1="BUY",(((J10/F3)-1)*-1),(J10/F3)-1)*100</f>
-        <v>17.009409082896</v>
+        <v>15.4315045030972</v>
       </c>
     </row>
     <row r="8" s="19" customFormat="1" spans="1:7">
@@ -2704,7 +2704,7 @@
       </c>
       <c r="E8" s="30">
         <f t="shared" si="1"/>
-        <v>73.3020237282878</v>
+        <v>119.701064516129</v>
       </c>
       <c r="F8" s="35">
         <f>IF($B$1="BUY",F7*(1-$B$5/100),F7*(1+$B$5/100))</f>
@@ -2712,7 +2712,7 @@
       </c>
       <c r="G8" s="32">
         <f t="shared" si="0"/>
-        <v>326.153369653477</v>
+        <v>532.603379243097</v>
       </c>
     </row>
     <row r="9" s="19" customFormat="1" spans="1:10">
@@ -2727,7 +2727,7 @@
       </c>
       <c r="E9" s="30">
         <f t="shared" si="1"/>
-        <v>84.297327287531</v>
+        <v>155.611383870968</v>
       </c>
       <c r="F9" s="35">
         <f>IF($B$1="BUY",F8*(1-$B$5/100),F8*(1+$B$5/100))</f>
@@ -2735,7 +2735,7 @@
       </c>
       <c r="G9" s="32">
         <f t="shared" si="0"/>
-        <v>382.577902603529</v>
+        <v>706.232080876347</v>
       </c>
       <c r="I9" s="27" t="s">
         <v>30</v>
@@ -2754,25 +2754,19 @@
       <c r="D10" s="34">
         <v>7</v>
       </c>
-      <c r="E10" s="30">
-        <f t="shared" si="1"/>
-        <v>96.9419263806606</v>
-      </c>
-      <c r="F10" s="35">
-        <f>IF($B$1="BUY",F9*(1-$B$5/100),F9*(1+$B$5/100))</f>
-        <v>4.6292032406266</v>
-      </c>
+      <c r="E10" s="30"/>
+      <c r="F10" s="35"/>
       <c r="G10" s="32">
         <f t="shared" ref="G10:G16" si="2">E10*F10</f>
-        <v>448.763879753939</v>
+        <v>0</v>
       </c>
       <c r="I10" s="43">
         <f>G18/E18</f>
-        <v>4.38150495375578</v>
+        <v>4.35892719972671</v>
       </c>
       <c r="J10" s="44">
         <f>IF(B1="BUY",((B4/G18)+1)*I10,((B4/-G18)+1)*I10)</f>
-        <v>4.71547918604071</v>
+        <v>4.65188963147482</v>
       </c>
     </row>
     <row r="11" s="19" customFormat="1" spans="1:7">
@@ -2839,7 +2833,7 @@
       <c r="G15" s="32"/>
       <c r="I15" s="33">
         <f>IF(B1="BUY",F3*(1-(J7)/100),F3*(1+(J7)/100))</f>
-        <v>4.71547918604071</v>
+        <v>4.65188963147482</v>
       </c>
     </row>
     <row r="16" s="19" customFormat="1" spans="4:9">
@@ -2860,7 +2854,7 @@
       <c r="E17" s="38"/>
       <c r="F17" s="39">
         <f>IF(B1="BUY",MIN(F3:F16)*(1-($B$5/3)/100),MAX(F3:F16)*(1+($B$5/3)/100))</f>
-        <v>4.66006459556411</v>
+        <v>4.56869077996481</v>
       </c>
       <c r="G17" s="40">
         <f t="shared" si="0"/>
@@ -2868,7 +2862,7 @@
       </c>
       <c r="I17" s="33">
         <f>IF(B1="BUY",(((I15/I10)-1)*-1),((I15/I10)-1))*100</f>
-        <v>7.62236345296481</v>
+        <v>6.72097555945603</v>
       </c>
       <c r="J17" s="43" t="str">
         <f>IF(B1="BUY","TIENE QUE SUBIR","TIENE QUE BAJAR")</f>
@@ -2879,12 +2873,12 @@
       <c r="D18" s="41"/>
       <c r="E18" s="41">
         <f>SUM(E3:E17)</f>
-        <v>505.72763905901</v>
+        <v>576.524433498759</v>
       </c>
       <c r="F18" s="41"/>
       <c r="G18" s="41">
         <f>SUM(G3:G17)</f>
-        <v>2215.84815578827</v>
+        <v>2513.02803448477</v>
       </c>
       <c r="H18" s="41"/>
       <c r="I18" s="47" t="s">
@@ -2894,7 +2888,7 @@
     <row r="19" s="19" customFormat="1" spans="9:9">
       <c r="I19" s="48">
         <f>G18/B3</f>
-        <v>1.31192904427962</v>
+        <v>1.48787923888974</v>
       </c>
     </row>
     <row r="20" s="19" customFormat="1"/>
@@ -3267,8 +3261,8 @@
   <sheetPr/>
   <dimension ref="B1:E7"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="4"/>

</xml_diff>

<commit_message>
variacion entre 3 y 10
</commit_message>
<xml_diff>
--- a/SANTA3/FORMULAss.xlsx
+++ b/SANTA3/FORMULAss.xlsx
@@ -141,13 +141,13 @@
     <t>margen ratio</t>
   </si>
   <si>
+    <t>BUY</t>
+  </si>
+  <si>
     <t>primer tp a 0.7 porciento</t>
   </si>
   <si>
     <t>porc distancia entre posicion y precio (se recomienda que sea al menos la mitad del porsentaje que soporta)</t>
-  </si>
-  <si>
-    <t>BUY</t>
   </si>
   <si>
     <t>Size</t>
@@ -359,12 +359,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="0.00000"/>
-    <numFmt numFmtId="177" formatCode="0.000000"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="0.000000"/>
+    <numFmt numFmtId="179" formatCode="0.00000"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -431,6 +431,13 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -440,7 +447,91 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -454,98 +545,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -614,7 +614,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -626,49 +698,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -686,19 +752,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -710,55 +770,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -770,25 +782,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1037,17 +1037,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1070,8 +1064,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1115,11 +1109,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1137,13 +1137,13 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1155,130 +1155,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1289,41 +1289,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1378,7 +1378,7 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2494,7 +2494,7 @@
   <dimension ref="A1:XFD24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44444444444444" defaultRowHeight="14.4"/>
@@ -2521,7 +2521,7 @@
         <v>11</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" s="19" customFormat="1" ht="15.15" spans="4:7">
@@ -2543,28 +2543,28 @@
         <v>17</v>
       </c>
       <c r="B3" s="28">
-        <v>1748.57</v>
+        <v>1754.18</v>
       </c>
       <c r="D3" s="29" t="s">
         <v>18</v>
       </c>
       <c r="E3" s="30">
         <f>G3/F3</f>
-        <v>136.447132266875</v>
+        <v>111.589058524173</v>
       </c>
       <c r="F3" s="31">
-        <v>2.563</v>
+        <v>3.144</v>
       </c>
       <c r="G3" s="32">
         <f>B8</f>
-        <v>349.714</v>
+        <v>350.836</v>
       </c>
       <c r="I3" s="27" t="s">
         <v>19</v>
       </c>
       <c r="J3" s="41">
         <f>IF(B1="BUY",((I10/J10)-1)*-100,((I10/J10)-1)*100)</f>
-        <v>-2.24409686827769</v>
+        <v>-2.04541417001616</v>
       </c>
     </row>
     <row r="4" s="19" customFormat="1" spans="1:10">
@@ -2573,29 +2573,29 @@
       </c>
       <c r="B4" s="33">
         <f>-B3*$B$10/100</f>
-        <v>-349.714</v>
+        <v>-350.836</v>
       </c>
       <c r="D4" s="34">
         <v>1</v>
       </c>
       <c r="E4" s="30">
         <f>E3</f>
-        <v>136.447132266875</v>
+        <v>111.589058524173</v>
       </c>
       <c r="F4" s="35">
         <f>IF($B$1="BUY",F3*(1-$B$5/100),F3*(1+$B$5/100))</f>
-        <v>2.606571</v>
+        <v>3.090552</v>
       </c>
       <c r="G4" s="32">
         <f t="shared" ref="G4:G17" si="0">E4*F4</f>
-        <v>355.659138</v>
+        <v>344.871788</v>
       </c>
       <c r="I4" s="27" t="s">
         <v>21</v>
       </c>
       <c r="J4" s="41">
         <f>E18</f>
-        <v>5481.4087762778</v>
+        <v>6140.08974692112</v>
       </c>
     </row>
     <row r="5" s="19" customFormat="1" spans="1:10">
@@ -2610,22 +2610,22 @@
       </c>
       <c r="E5" s="30">
         <f t="shared" ref="E4:E11" si="1">E4*(1+$B$6/100)</f>
-        <v>177.381271946937</v>
+        <v>145.065776081425</v>
       </c>
       <c r="F5" s="35">
         <f>IF($B$1="BUY",F4*(1-$B$5/100),F4*(1+$B$5/100))</f>
-        <v>2.650882707</v>
+        <v>3.038012616</v>
       </c>
       <c r="G5" s="32">
         <f t="shared" si="0"/>
-        <v>470.2169463498</v>
+        <v>440.7116578852</v>
       </c>
       <c r="I5" s="27" t="s">
         <v>23</v>
       </c>
       <c r="J5" s="41">
         <f>J4*J10</f>
-        <v>15583.730138548</v>
+        <v>17152.3207936528</v>
       </c>
     </row>
     <row r="6" s="19" customFormat="1" spans="1:10">
@@ -2640,22 +2640,22 @@
       </c>
       <c r="E6" s="30">
         <f t="shared" si="1"/>
-        <v>230.595653531018</v>
+        <v>188.585508905852</v>
       </c>
       <c r="F6" s="35">
         <f>IF($B$1="BUY",F5*(1-$B$5/100),F5*(1+$B$5/100))</f>
-        <v>2.695947713019</v>
+        <v>2.986366401528</v>
       </c>
       <c r="G6" s="32">
         <f t="shared" si="0"/>
-        <v>621.67382476907</v>
+        <v>563.185427611497</v>
       </c>
       <c r="I6" s="27" t="s">
         <v>25</v>
       </c>
       <c r="J6" s="41">
         <f>J3/100*J4*J10</f>
-        <v>-349.714000000001</v>
+        <v>-350.836000000002</v>
       </c>
     </row>
     <row r="7" s="19" customFormat="1" spans="1:10">
@@ -2670,22 +2670,22 @@
       </c>
       <c r="E7" s="30">
         <f t="shared" si="1"/>
-        <v>299.774349590324</v>
+        <v>245.161161577608</v>
       </c>
       <c r="F7" s="35">
         <f>IF($B$1="BUY",F6*(1-$B$5/100),F6*(1+$B$5/100))</f>
-        <v>2.74177882414032</v>
+        <v>2.93559817270202</v>
       </c>
       <c r="G7" s="32">
         <f t="shared" si="0"/>
-        <v>821.914963727188</v>
+        <v>719.694657944732</v>
       </c>
       <c r="I7" s="27" t="s">
         <v>27</v>
       </c>
       <c r="J7" s="42">
         <f>IF(B1="BUY",(((J10/F3)-1)*-1),(J10/F3)-1)*100</f>
-        <v>10.9253025633419</v>
+        <v>11.1483219890443</v>
       </c>
     </row>
     <row r="8" s="19" customFormat="1" spans="1:7">
@@ -2694,22 +2694,22 @@
       </c>
       <c r="B8" s="33">
         <f>B3*$B$9/100</f>
-        <v>349.714</v>
+        <v>350.836</v>
       </c>
       <c r="D8" s="34">
         <v>5</v>
       </c>
       <c r="E8" s="30">
         <f t="shared" si="1"/>
-        <v>389.706654467421</v>
+        <v>318.709510050891</v>
       </c>
       <c r="F8" s="35">
         <f>IF($B$1="BUY",F7*(1-$B$5/100),F7*(1+$B$5/100))</f>
-        <v>2.78838906415071</v>
+        <v>2.88569300376609</v>
       </c>
       <c r="G8" s="32">
         <f t="shared" si="0"/>
-        <v>1086.65377354372</v>
+        <v>919.697803387573</v>
       </c>
     </row>
     <row r="9" s="19" customFormat="1" spans="1:10">
@@ -2722,11 +2722,17 @@
       <c r="D9" s="34">
         <v>6</v>
       </c>
-      <c r="E9" s="30"/>
-      <c r="F9" s="35"/>
+      <c r="E9" s="30">
+        <f>E8*(1+$B$6/100)</f>
+        <v>414.322363066158</v>
+      </c>
+      <c r="F9" s="35">
+        <f>IF($B$1="BUY",F8*(1-$B$5/100),F8*(1+$B$5/100))</f>
+        <v>2.83663622270207</v>
+      </c>
       <c r="G9" s="32">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1175.28182294898</v>
       </c>
       <c r="I9" s="27" t="s">
         <v>30</v>
@@ -2753,20 +2759,20 @@
       </c>
       <c r="I10" s="43">
         <f>G18/E18</f>
-        <v>2.77921548279286</v>
+        <v>2.8506353351642</v>
       </c>
       <c r="J10" s="44">
         <f>IF(B1="BUY",((B4/G18)+1)*I10,((B4/-G18)+1)*I10)</f>
-        <v>2.84301550469845</v>
+        <v>2.79349675666445</v>
       </c>
     </row>
     <row r="11" s="19" customFormat="1" spans="1:7">
       <c r="A11" s="27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B11" s="33">
         <f>B8*0.7/100</f>
-        <v>2.447998</v>
+        <v>2.455852</v>
       </c>
       <c r="D11" s="34">
         <v>8</v>
@@ -2824,7 +2830,7 @@
       <c r="G15" s="32"/>
       <c r="I15" s="42">
         <f>IF(B1="BUY",F3*(1-(J7)/100),F3*(1+(J7)/100))</f>
-        <v>2.84301550469845</v>
+        <v>2.79349675666445</v>
       </c>
     </row>
     <row r="16" s="19" customFormat="1" spans="4:9">
@@ -2835,7 +2841,7 @@
       <c r="F16" s="35"/>
       <c r="G16" s="32"/>
       <c r="I16" s="47" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" s="19" customFormat="1" ht="18.15" spans="4:10">
@@ -2844,35 +2850,35 @@
       </c>
       <c r="E17" s="37">
         <f>SUM(E3:E9)*3</f>
-        <v>4111.05658220835</v>
+        <v>4605.06731019084</v>
       </c>
       <c r="F17" s="38">
         <f>IF(B1="BUY",MIN(F3:F16)*(1-($B$5/3)/100),MAX(F3:F16)*(1+($B$5/3)/100))</f>
-        <v>2.80418993551423</v>
+        <v>2.82056195077342</v>
       </c>
       <c r="G17" s="39">
         <f t="shared" si="0"/>
-        <v>11528.1834921582</v>
+        <v>12988.8776358748</v>
       </c>
       <c r="I17" s="42">
         <f>IF(B1="BUY",(((I15/I10)-1)*-1),((I15/I10)-1))*100</f>
-        <v>2.29561263963145</v>
+        <v>2.00441556992293</v>
       </c>
       <c r="J17" s="43" t="str">
         <f>IF(B1="BUY","TIENE QUE SUBIR","TIENE QUE BAJAR")</f>
-        <v>TIENE QUE BAJAR</v>
+        <v>TIENE QUE SUBIR</v>
       </c>
     </row>
     <row r="18" s="19" customFormat="1" spans="4:9">
       <c r="D18" s="40"/>
       <c r="E18" s="40">
         <f>SUM(E3:E17)</f>
-        <v>5481.4087762778</v>
+        <v>6140.08974692112</v>
       </c>
       <c r="F18" s="40"/>
       <c r="G18" s="40">
         <f>SUM(G3:G17)</f>
-        <v>15234.0161385479</v>
+        <v>17503.1567936528</v>
       </c>
       <c r="H18" s="40"/>
       <c r="I18" s="47" t="s">
@@ -2882,7 +2888,7 @@
     <row r="19" s="19" customFormat="1" spans="9:9">
       <c r="I19" s="48">
         <f>G18/B3</f>
-        <v>8.71227124939119</v>
+        <v>9.97797078615237</v>
       </c>
     </row>
     <row r="20" s="19" customFormat="1"/>
@@ -3030,7 +3036,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>

</xml_diff>

<commit_message>
vuelvo a estrategia original
</commit_message>
<xml_diff>
--- a/SANTA3/FORMULAss.xlsx
+++ b/SANTA3/FORMULAss.xlsx
@@ -141,13 +141,13 @@
     <t>margen ratio</t>
   </si>
   <si>
+    <t>primer tp a 0.7 porciento</t>
+  </si>
+  <si>
+    <t>porc distancia entre posicion y precio (se recomienda que sea al menos la mitad del porsentaje que soporta)</t>
+  </si>
+  <si>
     <t>BUY</t>
-  </si>
-  <si>
-    <t>primer tp a 0.7 porciento</t>
-  </si>
-  <si>
-    <t>porc distancia entre posicion y precio (se recomienda que sea al menos la mitad del porsentaje que soporta)</t>
   </si>
   <si>
     <t>Size</t>
@@ -359,11 +359,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="0.000000"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="0.000000"/>
     <numFmt numFmtId="179" formatCode="0.00000"/>
   </numFmts>
   <fonts count="27">
@@ -431,23 +431,17 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -455,37 +449,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -499,7 +462,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -507,33 +470,9 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -553,9 +492,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -568,8 +507,69 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -614,7 +614,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -626,25 +668,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -662,25 +704,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -692,73 +776,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -770,25 +788,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1033,39 +1033,6 @@
       </top>
       <bottom style="medium">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1088,18 +1055,31 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1120,32 +1100,52 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1155,130 +1155,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="24" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1289,41 +1289,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2494,7 +2494,7 @@
   <dimension ref="A1:XFD24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44444444444444" defaultRowHeight="14.4"/>
@@ -2521,7 +2521,7 @@
         <v>11</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" s="19" customFormat="1" ht="15.15" spans="4:7">
@@ -2543,28 +2543,28 @@
         <v>17</v>
       </c>
       <c r="B3" s="28">
-        <v>1929</v>
+        <v>2222.55</v>
       </c>
       <c r="D3" s="29" t="s">
         <v>18</v>
       </c>
       <c r="E3" s="30">
         <f>G3/F3</f>
-        <v>106.964847768893</v>
+        <v>26.1522621639113</v>
       </c>
       <c r="F3" s="31">
-        <v>9.016981</v>
+        <v>16.997</v>
       </c>
       <c r="G3" s="32">
         <f>B8</f>
-        <v>964.5</v>
+        <v>444.51</v>
       </c>
       <c r="I3" s="27" t="s">
         <v>19</v>
       </c>
       <c r="J3" s="41">
         <f>IF(B1="BUY",((I10/J10)-1)*-100,((I10/J10)-1)*100)</f>
-        <v>-1.90326229629663</v>
+        <v>-1.9856126430573</v>
       </c>
     </row>
     <row r="4" s="19" customFormat="1" spans="1:10">
@@ -2573,29 +2573,29 @@
       </c>
       <c r="B4" s="33">
         <f>-B3*$B$10/100</f>
-        <v>-964.5</v>
+        <v>-444.51</v>
       </c>
       <c r="D4" s="34">
         <v>1</v>
       </c>
       <c r="E4" s="30">
         <f>E3</f>
-        <v>106.964847768893</v>
+        <v>26.1522621639113</v>
       </c>
       <c r="F4" s="35">
         <f>IF($B$1="BUY",F3*(1-$B$5/100),F3*(1+$B$5/100))</f>
-        <v>8.863692323</v>
+        <v>17.285949</v>
       </c>
       <c r="G4" s="32">
         <f t="shared" ref="G4:G17" si="0">E4*F4</f>
-        <v>948.1035</v>
+        <v>452.06667</v>
       </c>
       <c r="I4" s="27" t="s">
         <v>21</v>
       </c>
       <c r="J4" s="41">
         <f>E18</f>
-        <v>6401.94550931182</v>
+        <v>1501.27967043868</v>
       </c>
     </row>
     <row r="5" s="19" customFormat="1" spans="1:10">
@@ -2609,23 +2609,23 @@
         <v>2</v>
       </c>
       <c r="E5" s="30">
-        <f>E4*(1+$B$6/100)</f>
-        <v>139.054302099561</v>
+        <f t="shared" ref="E5:E10" si="1">E4*(1+$B$6/100)</f>
+        <v>33.9979408130847</v>
       </c>
       <c r="F5" s="35">
         <f>IF($B$1="BUY",F4*(1-$B$5/100),F4*(1+$B$5/100))</f>
-        <v>8.713009553509</v>
+        <v>17.579810133</v>
       </c>
       <c r="G5" s="32">
         <f t="shared" si="0"/>
-        <v>1211.58146265</v>
+        <v>597.677344407</v>
       </c>
       <c r="I5" s="27" t="s">
         <v>23</v>
       </c>
       <c r="J5" s="41">
         <f>J4*J10</f>
-        <v>50676.1470490288</v>
+        <v>22386.5415822281</v>
       </c>
     </row>
     <row r="6" s="19" customFormat="1" spans="1:10">
@@ -2639,23 +2639,23 @@
         <v>3</v>
       </c>
       <c r="E6" s="30">
-        <f>E5*(1+$B$6/100)</f>
-        <v>180.770592729429</v>
+        <f t="shared" si="1"/>
+        <v>44.1973230570101</v>
       </c>
       <c r="F6" s="35">
         <f>IF($B$1="BUY",F5*(1-$B$5/100),F5*(1+$B$5/100))</f>
-        <v>8.56488839109934</v>
+        <v>17.878666905261</v>
       </c>
       <c r="G6" s="32">
         <f t="shared" si="0"/>
-        <v>1548.27995112043</v>
+        <v>790.189217040495</v>
       </c>
       <c r="I6" s="27" t="s">
         <v>25</v>
       </c>
       <c r="J6" s="41">
         <f>J3/100*J4*J10</f>
-        <v>-964.500000000001</v>
+        <v>-444.510000000001</v>
       </c>
     </row>
     <row r="7" s="19" customFormat="1" spans="1:10">
@@ -2669,23 +2669,23 @@
         <v>4</v>
       </c>
       <c r="E7" s="30">
-        <f>E6*(1+$B$6/100)</f>
-        <v>235.001770548258</v>
+        <f t="shared" si="1"/>
+        <v>57.4565199741131</v>
       </c>
       <c r="F7" s="35">
         <f>IF($B$1="BUY",F6*(1-$B$5/100),F6*(1+$B$5/100))</f>
-        <v>8.41928528845066</v>
+        <v>18.1826042426504</v>
       </c>
       <c r="G7" s="32">
         <f t="shared" si="0"/>
-        <v>1978.5469495368</v>
+        <v>1044.70916384924</v>
       </c>
       <c r="I7" s="27" t="s">
         <v>27</v>
       </c>
       <c r="J7" s="42">
         <f>IF(B1="BUY",(((J10/F3)-1)*-1),(J10/F3)-1)*100</f>
-        <v>12.2129490668851</v>
+        <v>-12.2689902230939</v>
       </c>
     </row>
     <row r="8" s="19" customFormat="1" spans="1:7">
@@ -2694,22 +2694,22 @@
       </c>
       <c r="B8" s="33">
         <f>B3*$B$9/100</f>
-        <v>964.5</v>
+        <v>444.51</v>
       </c>
       <c r="D8" s="34">
         <v>5</v>
       </c>
       <c r="E8" s="30">
-        <f>E7*(1+$B$6/100)</f>
-        <v>305.502301712735</v>
+        <f t="shared" si="1"/>
+        <v>74.693475966347</v>
       </c>
       <c r="F8" s="35">
         <f>IF($B$1="BUY",F7*(1-$B$5/100),F7*(1+$B$5/100))</f>
-        <v>8.27615743854699</v>
+        <v>18.4917085147755</v>
       </c>
       <c r="G8" s="32">
         <f t="shared" si="0"/>
-        <v>2528.38514681308</v>
+        <v>1381.20998552508</v>
       </c>
     </row>
     <row r="9" s="19" customFormat="1" spans="1:10">
@@ -2717,22 +2717,22 @@
         <v>29</v>
       </c>
       <c r="B9" s="28">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="D9" s="34">
         <v>6</v>
       </c>
       <c r="E9" s="30">
-        <f>E8*(1+$B$6/100)</f>
-        <v>397.152992226556</v>
+        <f t="shared" si="1"/>
+        <v>97.1015187562511</v>
       </c>
       <c r="F9" s="35">
         <f>IF($B$1="BUY",F8*(1-$B$5/100),F8*(1+$B$5/100))</f>
-        <v>8.1354627620917</v>
+        <v>18.8060675595267</v>
       </c>
       <c r="G9" s="32">
         <f t="shared" si="0"/>
-        <v>3231.02337911244</v>
+        <v>1826.0977218627</v>
       </c>
       <c r="I9" s="27" t="s">
         <v>30</v>
@@ -2746,70 +2746,88 @@
         <v>32</v>
       </c>
       <c r="B10" s="28">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="D10" s="34">
         <v>7</v>
       </c>
       <c r="E10" s="30">
-        <f>E9*(1+$B$6/100)</f>
-        <v>516.298889894523</v>
+        <f t="shared" si="1"/>
+        <v>126.231974383126</v>
       </c>
       <c r="F10" s="35">
         <f>IF($B$1="BUY",F9*(1-$B$5/100),F9*(1+$B$5/100))</f>
-        <v>7.99715989513614</v>
+        <v>19.1257707080386</v>
       </c>
       <c r="G10" s="32">
-        <f t="shared" ref="G10:G16" si="1">E10*F10</f>
-        <v>4128.92477616778</v>
+        <f t="shared" ref="G10:G16" si="2">E10*F10</f>
+        <v>2414.28379807468</v>
       </c>
       <c r="I10" s="43">
         <f>G18/E18</f>
-        <v>8.06639903040661</v>
+        <v>14.6155523279793</v>
       </c>
       <c r="J10" s="44">
         <f>IF(B1="BUY",((B4/G18)+1)*I10,((B4/-G18)+1)*I10)</f>
-        <v>7.91574170309929</v>
+        <v>14.9116397317807</v>
       </c>
     </row>
     <row r="11" s="19" customFormat="1" spans="1:7">
       <c r="A11" s="27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" s="33">
         <f>B8*0.7/100</f>
-        <v>6.7515</v>
+        <v>3.11157</v>
       </c>
       <c r="D11" s="34">
         <v>8</v>
       </c>
-      <c r="E11" s="30"/>
-      <c r="F11" s="35"/>
+      <c r="E11" s="30">
+        <f>E10*(1+$B$6/100)</f>
+        <v>164.101566698064</v>
+      </c>
+      <c r="F11" s="35">
+        <f>IF($B$1="BUY",F10*(1-$B$5/100),F10*(1+$B$5/100))</f>
+        <v>19.4509088100753</v>
+      </c>
       <c r="G11" s="32">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>3191.92460943454</v>
       </c>
     </row>
     <row r="12" s="19" customFormat="1" spans="4:7">
       <c r="D12" s="34">
         <v>9</v>
       </c>
-      <c r="E12" s="30"/>
-      <c r="F12" s="35"/>
+      <c r="E12" s="30">
+        <f>E11*(1+$B$6/100)</f>
+        <v>213.332036707484</v>
+      </c>
+      <c r="F12" s="35">
+        <f>IF($B$1="BUY",F11*(1-$B$5/100),F11*(1+$B$5/100))</f>
+        <v>19.7815742598466</v>
+      </c>
       <c r="G12" s="32">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>4220.0435261334</v>
       </c>
     </row>
     <row r="13" s="19" customFormat="1" spans="4:10">
       <c r="D13" s="34">
         <v>10</v>
       </c>
-      <c r="E13" s="30"/>
-      <c r="F13" s="35"/>
+      <c r="E13" s="30">
+        <f>E12*(1+$B$6/100)</f>
+        <v>277.331647719729</v>
+      </c>
+      <c r="F13" s="35">
+        <f>IF($B$1="BUY",F12*(1-$B$5/100),F12*(1+$B$5/100))</f>
+        <v>20.1178610222639</v>
+      </c>
       <c r="G13" s="32">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>5579.31954590097</v>
       </c>
       <c r="I13" s="45" t="s">
         <v>33</v>
@@ -2820,8 +2838,14 @@
       <c r="D14" s="34">
         <v>11</v>
       </c>
-      <c r="E14" s="30"/>
-      <c r="F14" s="35"/>
+      <c r="E14" s="30">
+        <f>E13*(1+$B$6/100)</f>
+        <v>360.531142035648</v>
+      </c>
+      <c r="F14" s="35">
+        <f>IF($B$1="BUY",F13*(1-$B$5/100),F13*(1+$B$5/100))</f>
+        <v>20.4598646596424</v>
+      </c>
       <c r="G14" s="32"/>
       <c r="I14" s="46" t="s">
         <v>34</v>
@@ -2836,7 +2860,7 @@
       <c r="G15" s="32"/>
       <c r="I15" s="42">
         <f>IF(B1="BUY",F3*(1-(J7)/100),F3*(1+(J7)/100))</f>
-        <v>7.91574170309929</v>
+        <v>14.9116397317807</v>
       </c>
     </row>
     <row r="16" s="19" customFormat="1" spans="4:9">
@@ -2847,44 +2871,41 @@
       <c r="F16" s="35"/>
       <c r="G16" s="32"/>
       <c r="I16" s="47" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" s="19" customFormat="1" ht="18.15" spans="4:10">
       <c r="D17" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="37">
-        <f>SUM(E3:E9)*3</f>
-        <v>4414.23496456297</v>
-      </c>
+      <c r="E17" s="37"/>
       <c r="F17" s="38">
         <f>IF(B1="BUY",MIN(F3:F16)*(1-($B$5/3)/100),MAX(F3:F16)*(1+($B$5/3)/100))</f>
-        <v>7.95184265573036</v>
+        <v>20.5758038927137</v>
       </c>
       <c r="G17" s="39">
         <f t="shared" si="0"/>
-        <v>35101.3018836283</v>
+        <v>0</v>
       </c>
       <c r="I17" s="42">
         <f>IF(B1="BUY",(((I15/I10)-1)*-1),((I15/I10)-1))*100</f>
-        <v>1.86771478499153</v>
+        <v>2.02583793726754</v>
       </c>
       <c r="J17" s="43" t="str">
         <f>IF(B1="BUY","TIENE QUE SUBIR","TIENE QUE BAJAR")</f>
-        <v>TIENE QUE SUBIR</v>
+        <v>TIENE QUE BAJAR</v>
       </c>
     </row>
     <row r="18" s="19" customFormat="1" spans="4:9">
       <c r="D18" s="40"/>
       <c r="E18" s="40">
         <f>SUM(E3:E17)</f>
-        <v>6401.94550931182</v>
+        <v>1501.27967043868</v>
       </c>
       <c r="F18" s="40"/>
       <c r="G18" s="40">
         <f>SUM(G3:G17)</f>
-        <v>51640.6470490288</v>
+        <v>21942.0315822281</v>
       </c>
       <c r="H18" s="40"/>
       <c r="I18" s="47" t="s">
@@ -2894,7 +2915,7 @@
     <row r="19" s="19" customFormat="1" spans="9:9">
       <c r="I19" s="48">
         <f>G18/B3</f>
-        <v>26.7706827625862</v>
+        <v>9.87245802444404</v>
       </c>
     </row>
     <row r="20" s="19" customFormat="1"/>
@@ -3042,7 +3063,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>

</xml_diff>

<commit_message>
apalancamiento de 30 para poder generar ataque
</commit_message>
<xml_diff>
--- a/SANTA3/FORMULAss.xlsx
+++ b/SANTA3/FORMULAss.xlsx
@@ -132,7 +132,7 @@
     <t>distancia entre posicion y precio</t>
   </si>
   <si>
-    <t>ataque seria =SUM(E3:E9)*3</t>
+    <t>ataque seria =SUM(E3:E16)*3</t>
   </si>
   <si>
     <t>ataque</t>
@@ -141,13 +141,13 @@
     <t>margen ratio</t>
   </si>
   <si>
+    <t>BUY</t>
+  </si>
+  <si>
     <t>primer tp a 0.7 porciento</t>
   </si>
   <si>
     <t>porc distancia entre posicion y precio (se recomienda que sea al menos la mitad del porsentaje que soporta)</t>
-  </si>
-  <si>
-    <t>BUY</t>
   </si>
   <si>
     <t>Size</t>
@@ -359,12 +359,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="0.000000"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="0.00000"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="0.00000"/>
+    <numFmt numFmtId="179" formatCode="0.000000"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -432,22 +432,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -460,40 +445,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -507,46 +460,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -568,8 +492,84 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -614,37 +614,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -656,25 +638,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -692,7 +668,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -704,13 +746,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -722,73 +788,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1037,6 +1037,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1046,17 +1061,28 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1086,16 +1112,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1108,177 +1134,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1289,41 +1289,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1378,7 +1378,7 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2494,7 +2494,7 @@
   <dimension ref="A1:XFD24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:F3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44444444444444" defaultRowHeight="14.4"/>
@@ -2521,7 +2521,7 @@
         <v>11</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" s="19" customFormat="1" ht="15.15" spans="4:7">
@@ -2543,28 +2543,28 @@
         <v>17</v>
       </c>
       <c r="B3" s="28">
-        <v>2264.78</v>
+        <v>1932.25</v>
       </c>
       <c r="D3" s="29" t="s">
         <v>18</v>
       </c>
       <c r="E3" s="30">
         <f>G3/F3</f>
-        <v>716.249209361164</v>
+        <v>16.1235814419226</v>
       </c>
       <c r="F3" s="31">
-        <v>0.3162</v>
+        <v>5.992</v>
       </c>
       <c r="G3" s="32">
         <f>B8</f>
-        <v>226.478</v>
+        <v>96.6125</v>
       </c>
       <c r="I3" s="27" t="s">
         <v>19</v>
       </c>
       <c r="J3" s="41">
         <f>IF(B1="BUY",((I10/J10)-1)*-100,((I10/J10)-1)*100)</f>
-        <v>-1.47414326889548</v>
+        <v>-1.83361453335968</v>
       </c>
     </row>
     <row r="4" s="19" customFormat="1" spans="1:10">
@@ -2573,29 +2573,29 @@
       </c>
       <c r="B4" s="33">
         <f>-B3*$B$10/100</f>
-        <v>-226.478</v>
+        <v>-193.225</v>
       </c>
       <c r="D4" s="34">
         <v>1</v>
       </c>
       <c r="E4" s="30">
         <f>E3</f>
-        <v>716.249209361164</v>
+        <v>16.1235814419226</v>
       </c>
       <c r="F4" s="35">
         <f>IF($B$1="BUY",F3*(1-$B$5/100),F3*(1+$B$5/100))</f>
-        <v>0.3215754</v>
+        <v>5.87216</v>
       </c>
       <c r="G4" s="32">
         <f t="shared" ref="G4:G17" si="0">E4*F4</f>
-        <v>230.328126</v>
+        <v>94.68025</v>
       </c>
       <c r="I4" s="27" t="s">
         <v>21</v>
       </c>
       <c r="J4" s="41">
         <f>E18</f>
-        <v>42868.1805757812</v>
+        <v>2129.28003042715</v>
       </c>
     </row>
     <row r="5" s="19" customFormat="1" spans="1:10">
@@ -2603,29 +2603,29 @@
         <v>22</v>
       </c>
       <c r="B5" s="33">
-        <v>1.7</v>
+        <v>2</v>
       </c>
       <c r="D5" s="34">
         <v>2</v>
       </c>
       <c r="E5" s="30">
         <f t="shared" ref="E5:E14" si="1">E4*(1+$B$6/100)</f>
-        <v>931.123972169513</v>
+        <v>20.9606558744993</v>
       </c>
       <c r="F5" s="35">
         <f>IF($B$1="BUY",F4*(1-$B$5/100),F4*(1+$B$5/100))</f>
-        <v>0.3270421818</v>
+        <v>5.7547168</v>
       </c>
       <c r="G5" s="32">
         <f t="shared" si="0"/>
-        <v>304.5168153846</v>
+        <v>120.6226385</v>
       </c>
       <c r="I5" s="27" t="s">
         <v>23</v>
       </c>
       <c r="J5" s="41">
         <f>J4*J10</f>
-        <v>15363.3642522202</v>
+        <v>10537.9291276645</v>
       </c>
     </row>
     <row r="6" s="19" customFormat="1" spans="1:10">
@@ -2640,22 +2640,22 @@
       </c>
       <c r="E6" s="30">
         <f t="shared" si="1"/>
-        <v>1210.46116382037</v>
+        <v>27.2488526368491</v>
       </c>
       <c r="F6" s="35">
         <f>IF($B$1="BUY",F5*(1-$B$5/100),F5*(1+$B$5/100))</f>
-        <v>0.3326018988906</v>
+        <v>5.639622464</v>
       </c>
       <c r="G6" s="32">
         <f t="shared" si="0"/>
-        <v>402.60168161998</v>
+        <v>153.673241449</v>
       </c>
       <c r="I6" s="27" t="s">
         <v>25</v>
       </c>
       <c r="J6" s="41">
         <f>J3/100*J4*J10</f>
-        <v>-226.477999999998</v>
+        <v>-193.225</v>
       </c>
     </row>
     <row r="7" s="19" customFormat="1" spans="1:10">
@@ -2670,22 +2670,22 @@
       </c>
       <c r="E7" s="30">
         <f t="shared" si="1"/>
-        <v>1573.59951296648</v>
+        <v>35.4235084279039</v>
       </c>
       <c r="F7" s="35">
         <f>IF($B$1="BUY",F6*(1-$B$5/100),F6*(1+$B$5/100))</f>
-        <v>0.33825613117174</v>
+        <v>5.52683001472</v>
       </c>
       <c r="G7" s="32">
         <f t="shared" si="0"/>
-        <v>532.279683269775</v>
+        <v>195.779709606026</v>
       </c>
       <c r="I7" s="27" t="s">
         <v>27</v>
       </c>
       <c r="J7" s="42">
         <f>IF(B1="BUY",(((J10/F3)-1)*-1),(J10/F3)-1)*100</f>
-        <v>13.3416185994296</v>
+        <v>17.4055838267995</v>
       </c>
     </row>
     <row r="8" s="19" customFormat="1" spans="1:7">
@@ -2694,22 +2694,22 @@
       </c>
       <c r="B8" s="33">
         <f>B3*$B$9/100</f>
-        <v>226.478</v>
+        <v>96.6125</v>
       </c>
       <c r="D8" s="34">
         <v>5</v>
       </c>
       <c r="E8" s="30">
         <f t="shared" si="1"/>
-        <v>2045.67936685642</v>
+        <v>46.050560956275</v>
       </c>
       <c r="F8" s="35">
         <f>IF($B$1="BUY",F7*(1-$B$5/100),F7*(1+$B$5/100))</f>
-        <v>0.34400648540166</v>
+        <v>5.4162934144256</v>
       </c>
       <c r="G8" s="32">
         <f t="shared" si="0"/>
-        <v>703.72696925097</v>
+        <v>249.423350038077</v>
       </c>
     </row>
     <row r="9" s="19" customFormat="1" spans="1:10">
@@ -2717,22 +2717,22 @@
         <v>29</v>
       </c>
       <c r="B9" s="28">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D9" s="34">
         <v>6</v>
       </c>
       <c r="E9" s="30">
         <f t="shared" si="1"/>
-        <v>2659.38317691335</v>
+        <v>59.8657292431576</v>
       </c>
       <c r="F9" s="35">
         <f>IF($B$1="BUY",F8*(1-$B$5/100),F8*(1+$B$5/100))</f>
-        <v>0.349854595653488</v>
+        <v>5.30796754613709</v>
       </c>
       <c r="G9" s="32">
         <f t="shared" si="0"/>
-        <v>930.397426046707</v>
+        <v>317.76534794851</v>
       </c>
       <c r="I9" s="27" t="s">
         <v>30</v>
@@ -2753,52 +2753,64 @@
       </c>
       <c r="E10" s="30">
         <f t="shared" si="1"/>
-        <v>3457.19812998735</v>
+        <v>77.8254480161048</v>
       </c>
       <c r="F10" s="35">
         <f>IF($B$1="BUY",F9*(1-$B$5/100),F9*(1+$B$5/100))</f>
-        <v>0.355802123779597</v>
+        <v>5.20180819521435</v>
       </c>
       <c r="G10" s="32">
         <f t="shared" ref="G10:G16" si="2">E10*F10</f>
-        <v>1230.07843697635</v>
+        <v>404.833053286402</v>
       </c>
       <c r="I10" s="43">
         <f>G18/E18</f>
-        <v>0.353103071996761</v>
+        <v>5.0398040531624</v>
       </c>
       <c r="J10" s="44">
         <f>IF(B1="BUY",((B4/G18)+1)*I10,((B4/-G18)+1)*I10)</f>
-        <v>0.358386198011396</v>
+        <v>4.94905741709817</v>
       </c>
     </row>
     <row r="11" s="19" customFormat="1" spans="1:7">
       <c r="A11" s="27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B11" s="33">
         <f>B8*0.7/100</f>
-        <v>1.585346</v>
+        <v>0.6762875</v>
       </c>
       <c r="D11" s="34">
         <v>8</v>
       </c>
-      <c r="E11" s="30"/>
-      <c r="F11" s="35"/>
+      <c r="E11" s="30">
+        <f>E10*(1+$B$6/100)</f>
+        <v>101.173082420936</v>
+      </c>
+      <c r="F11" s="35">
+        <f>IF($B$1="BUY",F10*(1-$B$5/100),F10*(1+$B$5/100))</f>
+        <v>5.09777203131006</v>
+      </c>
       <c r="G11" s="32">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>515.757309886876</v>
       </c>
     </row>
     <row r="12" s="19" customFormat="1" spans="4:7">
       <c r="D12" s="34">
         <v>9</v>
       </c>
-      <c r="E12" s="30"/>
-      <c r="F12" s="35"/>
+      <c r="E12" s="30">
+        <f>E11*(1+$B$6/100)</f>
+        <v>131.525007147217</v>
+      </c>
+      <c r="F12" s="35">
+        <f>IF($B$1="BUY",F11*(1-$B$5/100),F11*(1+$B$5/100))</f>
+        <v>4.99581659068386</v>
+      </c>
       <c r="G12" s="32">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>657.07481279588</v>
       </c>
     </row>
     <row r="13" s="19" customFormat="1" spans="4:10">
@@ -2836,7 +2848,7 @@
       <c r="G15" s="32"/>
       <c r="I15" s="42">
         <f>IF(B1="BUY",F3*(1-(J7)/100),F3*(1+(J7)/100))</f>
-        <v>0.358386198011396</v>
+        <v>4.94905741709817</v>
       </c>
     </row>
     <row r="16" s="19" customFormat="1" spans="4:9">
@@ -2847,7 +2859,7 @@
       <c r="F16" s="35"/>
       <c r="G16" s="32"/>
       <c r="I16" s="47" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" s="19" customFormat="1" ht="18.15" spans="4:10">
@@ -2855,36 +2867,36 @@
         <v>37</v>
       </c>
       <c r="E17" s="37">
-        <f>SUM(E3:E9)*3</f>
-        <v>29558.2368343454</v>
+        <f>SUM(E3:E16)*3</f>
+        <v>1596.96002282036</v>
       </c>
       <c r="F17" s="38">
         <f>IF(B1="BUY",MIN(F3:F16)*(1-($B$5/3)/100),MAX(F3:F16)*(1+($B$5/3)/100))</f>
-        <v>0.357818335814348</v>
+        <v>4.96251114674596</v>
       </c>
       <c r="G17" s="39">
         <f t="shared" si="0"/>
-        <v>10576.4791136718</v>
+        <v>7924.93191415375</v>
       </c>
       <c r="I17" s="42">
         <f>IF(B1="BUY",(((I15/I10)-1)*-1),((I15/I10)-1))*100</f>
-        <v>1.49619939151475</v>
+        <v>1.80059849761987</v>
       </c>
       <c r="J17" s="43" t="str">
         <f>IF(B1="BUY","TIENE QUE SUBIR","TIENE QUE BAJAR")</f>
-        <v>TIENE QUE BAJAR</v>
+        <v>TIENE QUE SUBIR</v>
       </c>
     </row>
     <row r="18" s="19" customFormat="1" spans="4:9">
       <c r="D18" s="40"/>
       <c r="E18" s="40">
         <f>SUM(E3:E17)</f>
-        <v>42868.1805757812</v>
+        <v>2129.28003042715</v>
       </c>
       <c r="F18" s="40"/>
       <c r="G18" s="40">
         <f>SUM(G3:G17)</f>
-        <v>15136.8862522202</v>
+        <v>10731.1541276645</v>
       </c>
       <c r="H18" s="40"/>
       <c r="I18" s="47" t="s">
@@ -2894,7 +2906,7 @@
     <row r="19" s="19" customFormat="1" spans="9:9">
       <c r="I19" s="48">
         <f>G18/B3</f>
-        <v>6.68360116753954</v>
+        <v>5.55370895467177</v>
       </c>
     </row>
     <row r="20" s="19" customFormat="1"/>
@@ -3042,7 +3054,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>

</xml_diff>